<commit_message>
Correct fraction oxidized for liquid fuel to match Boden et al 1995 value
</commit_message>
<xml_diff>
--- a/input/default-emissions-data/CO2_base_EF.xlsx
+++ b/input/default-emissions-data/CO2_base_EF.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6345" yWindow="0" windowWidth="19320" windowHeight="13935" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="25600" windowHeight="13120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="EIA" sheetId="4" r:id="rId3"/>
     <sheet name="conversion" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="99">
   <si>
     <t>cdiac_fuel</t>
   </si>
@@ -60,9 +60,6 @@
     <t>coal_coke</t>
   </si>
   <si>
-    <t>http://cdiac.ornl.gov/pns/convert.html</t>
-  </si>
-  <si>
     <t>https://www.eia.gov/environment/emissions/co2_vol_mass.cfm</t>
   </si>
   <si>
@@ -318,10 +315,10 @@
     <t>Fraction oxidized</t>
   </si>
   <si>
-    <t>Source: http://cdiac.ornl.gov/pns/convert.html; http://cdiac.ornl.gov/epubs/ndp/ndp030/tables/table4.htm</t>
-  </si>
-  <si>
     <t>personal correspondence, also http://cdiac.ornl.gov/pns/convert.html</t>
+  </si>
+  <si>
+    <t>Source: http://cdiac.ornl.gov/epubs/ndp/ndp030/tables/table4.htm</t>
   </si>
 </sst>
 </file>
@@ -523,7 +520,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="52">
+  <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -580,6 +577,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -676,7 +675,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="52">
+  <cellStyles count="54">
     <cellStyle name="Body: normal cell" xfId="25"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -706,6 +705,8 @@
     <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="Font: Calibri, 9pt regular" xfId="30"/>
     <cellStyle name="Footnotes: all except top row" xfId="31"/>
     <cellStyle name="Footnotes: top row" xfId="28"/>
@@ -1065,15 +1066,15 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1090,7 +1091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -1103,26 +1104,26 @@
         <v>kt CO2/kJ</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3">
         <f>CDIAC!E3</f>
-        <v>3.0676840000000003</v>
+        <v>3.0676839999999999</v>
       </c>
       <c r="D3" s="1" t="str">
         <f>CDIAC!F3</f>
         <v>kt CO2/kt</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -1135,10 +1136,10 @@
         <v>kt CO2/TJ</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -1151,10 +1152,10 @@
         <v>kt CO2/kt</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -1167,10 +1168,10 @@
         <v>kt CO2/TJ</v>
       </c>
       <c r="E6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1183,60 +1184,60 @@
         <v>kt CO2/kt</v>
       </c>
       <c r="E7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8">
         <f>EIA!J19</f>
-        <v>4.0271495041319945</v>
+        <v>4.3210700017102557</v>
       </c>
       <c r="D8" t="str">
         <f>EIA!K19</f>
         <v>kt CO2/kt</v>
       </c>
       <c r="E8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9">
         <f>EIA!J8</f>
-        <v>2.9686974479366599</v>
+        <v>3.1853670873830175</v>
       </c>
       <c r="D9" t="str">
         <f>EIA!K8</f>
         <v>kt CO2/kt</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10">
         <f>EIA!J12</f>
-        <v>2.8746886954186661</v>
+        <v>3.084497129615889</v>
       </c>
       <c r="D10" t="str">
         <f>EIA!K12</f>
         <v>kt CO2/kt</v>
       </c>
       <c r="E10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11">
         <f>EIA!J15</f>
@@ -1247,7 +1248,7 @@
         <v>kt CO2/kt</v>
       </c>
       <c r="E11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1265,20 +1266,20 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -1290,7 +1291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1298,109 +1299,112 @@
         <v>0.72409999999999997</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1">
         <f>B2*conversion!B5/conversion!B6</f>
         <v>9.0526088796080198E-11</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.83725000000000005</v>
+        <f>0.85*conversion!B21</f>
+        <v>0.83724999999999994</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <f>B3*conversion!B5</f>
-        <v>3.0676840000000003</v>
+        <v>3.0676839999999999</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
+        <f>0.0137*conversion!B22</f>
         <v>1.3426E-2</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4">
         <f>B4*conversion!B5</f>
         <v>4.9192864000000003E-2</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
+        <f>0.855*conversion!B23</f>
         <v>0.85499999999999998</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <f>B5*conversion!B5</f>
         <v>3.1327199999999999</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
+        <f>13.454*conversion!B24</f>
         <v>13.454000000000001</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <f>B6*conversion!B5/1000</f>
         <v>4.9295456000000001E-2</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="D9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1413,27 +1417,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19" style="3" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="17" customWidth="1"/>
-    <col min="7" max="7" width="11.625" style="17" customWidth="1"/>
-    <col min="8" max="9" width="8.875" style="3"/>
-    <col min="10" max="11" width="8.875" style="18"/>
-    <col min="12" max="16384" width="8.875" style="3"/>
+    <col min="7" max="7" width="11.6640625" style="17" customWidth="1"/>
+    <col min="8" max="9" width="8.83203125" style="3"/>
+    <col min="10" max="11" width="8.83203125" style="18"/>
+    <col min="12" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="18.75" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -1442,45 +1446,45 @@
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
     </row>
-    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="30" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="27.75" customHeight="1" thickBot="1">
+      <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" thickTop="1">
+      <c r="A4" s="29" t="s">
         <v>27</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>28</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
@@ -1489,22 +1493,22 @@
       <c r="F4" s="29"/>
       <c r="G4" s="29"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="10">
         <v>12.7</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="10">
         <f t="shared" ref="D5:D13" si="0">B5/2.20462</f>
         <v>5.7606299498326248</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="10">
         <v>139.04859867504859</v>
@@ -1514,22 +1518,22 @@
         <v>63.071458425963932</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="10">
         <v>14.8</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="10">
         <f t="shared" si="0"/>
         <v>6.7131750596474689</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="10">
         <v>143.19829002512873</v>
@@ -1539,22 +1543,22 @@
         <v>64.953728998706694</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15" customHeight="1">
       <c r="A7" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="10">
         <v>13.7</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="10">
         <f t="shared" si="0"/>
         <v>6.214222859268264</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="10">
         <v>141.12344435008868</v>
@@ -1564,22 +1568,22 @@
         <v>64.012593712335317</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="26.25" customHeight="1">
       <c r="A8" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="10">
         <v>22.4</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="10">
         <f t="shared" si="0"/>
         <v>10.160481171358329</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="10">
         <v>161.30000000000001</v>
@@ -1589,32 +1593,32 @@
         <v>73.164536291968702</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J8" s="18">
         <f>D8*conversion!B21/conversion!C13</f>
-        <v>2.9686974479366599</v>
+        <v>3.1853670873830175</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="10">
         <v>21.5</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="10">
         <f t="shared" si="0"/>
         <v>9.7522475528662547</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="10">
         <v>159.4</v>
@@ -1624,22 +1628,22 @@
         <v>72.302709764040983</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="10">
         <v>4631.5</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="10">
         <f t="shared" si="0"/>
         <v>2100.8155600511654</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="10">
         <v>210.2</v>
@@ -1649,22 +1653,22 @@
         <v>95.345229563371475</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="25">
       <c r="A11" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="10">
         <v>117.1</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="10">
         <f t="shared" si="0"/>
         <v>53.115729694913412</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="10">
         <v>117</v>
@@ -1674,22 +1678,22 @@
         <v>53.070370403969847</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15" customHeight="1">
       <c r="A12" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="10">
         <v>19.600000000000001</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="10">
         <f t="shared" si="0"/>
         <v>8.89042102493854</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="10">
         <v>157.19999999999999</v>
@@ -1698,32 +1702,32 @@
         <v>71.3</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J12" s="18">
         <f>D12*conversion!B21/conversion!C14</f>
-        <v>2.8746886954186661</v>
+        <v>3.084497129615889</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="25">
       <c r="A13" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="10">
         <v>26</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="10">
         <f t="shared" si="0"/>
         <v>11.793415645326633</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="10">
         <v>173.7</v>
@@ -1733,9 +1737,9 @@
         <v>78.789088368970624</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1">
       <c r="A14" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="30"/>
       <c r="C14" s="30"/>
@@ -1744,22 +1748,22 @@
       <c r="F14" s="30"/>
       <c r="G14" s="30"/>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15" customHeight="1">
       <c r="A15" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="10">
         <v>21.1</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="10">
         <f>B15/2.20462</f>
         <v>9.5708103890919993</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" s="10">
         <v>156.30000000000001</v>
@@ -1769,32 +1773,32 @@
         <v>70.896571744790492</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J15" s="18">
         <f>D15*conversion!B23/conversion!C13</f>
         <v>3.0461949575680598</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="10">
         <v>18.399999999999999</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="10">
         <f>B16/2.20462</f>
         <v>8.3461095336157705</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="10">
         <v>152.6</v>
@@ -1803,9 +1807,9 @@
         <v>69.2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1">
       <c r="A17" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
@@ -1814,22 +1818,22 @@
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
     </row>
-    <row r="18" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="22.5" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="10">
         <v>120.7</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="10">
         <f>B18/2.20462</f>
         <v>54.748664168881717</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F18" s="10">
         <v>120.6</v>
@@ -1839,22 +1843,22 @@
         <v>54.703304877938152</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="10">
         <v>32.4</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="10">
         <f>B19/2.20462</f>
         <v>14.696410265714727</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F19" s="10">
         <v>225.1</v>
@@ -1864,33 +1868,33 @@
         <v>102.10376391396251</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J19" s="18">
         <f>D19*conversion!B21/conversion!C12</f>
-        <v>4.0271495041319945</v>
+        <v>4.3210700017102557</v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="25">
       <c r="A20" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="10">
         <f>F20*5.796/42</f>
         <v>22.093800000000002</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="10">
         <f>B20/2.20462</f>
         <v>10.021591022489138</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F20" s="10">
         <v>160.1</v>
@@ -1900,9 +1904,9 @@
         <v>72.620224800645914</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1">
       <c r="A21" s="30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="30"/>
       <c r="C21" s="30"/>
@@ -1911,23 +1915,23 @@
       <c r="F21" s="30"/>
       <c r="G21" s="30"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="10">
         <f>F22*6.636/42</f>
         <v>26.3386</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" s="10">
         <f>B22/2.20462</f>
         <v>11.94700220446154</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F22" s="10">
         <v>166.7</v>
@@ -1937,23 +1941,23 @@
         <v>75.613938002921145</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="10">
         <f>F23*6.065/42</f>
         <v>23.624619047619049</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" s="10">
         <f>B23/2.20462</f>
         <v>10.715959688118158</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F23" s="10">
         <v>163.6</v>
@@ -1964,23 +1968,23 @@
       </c>
       <c r="K23" s="23"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="10">
         <f>F24*6.636/42</f>
         <v>24.742799999999999</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="10">
         <f>B24/2.20462</f>
         <v>11.223158639584147</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F24" s="10">
         <v>156.6</v>
@@ -1990,23 +1994,23 @@
         <v>71.032649617621175</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="10">
         <f>F25*5.248/42</f>
         <v>20.054857142857145</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25" s="10">
         <f>B25/2.20462</f>
         <v>9.0967409997446946</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F25" s="10">
         <v>160.5</v>
@@ -2016,23 +2020,23 @@
         <v>72.801661964420177</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="10">
         <f>F26*5.537/42</f>
         <v>21.106516666666668</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="10">
         <f>B26/2.20462</f>
         <v>9.5737663028851543</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F26" s="10">
         <v>160.1</v>
@@ -2042,9 +2046,9 @@
         <v>72.620224800645914</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1">
       <c r="A27" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" s="31"/>
       <c r="C27" s="31"/>
@@ -2053,22 +2057,22 @@
       <c r="F27" s="31"/>
       <c r="G27" s="31"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="10">
         <v>5685</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D28" s="10">
         <f>B28/2.20462</f>
         <v>2578.675690141612</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F28" s="10">
         <v>228.6</v>
@@ -2077,22 +2081,22 @@
         <v>103.7</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="10">
         <v>4931.3</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" s="10">
         <f>B29/2.20462</f>
         <v>2236.8027142999704</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F29" s="10">
         <v>205.7</v>
@@ -2101,22 +2105,22 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" s="10">
         <v>3715.9</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30" s="10">
         <f>B30/2.20462</f>
         <v>1685.5058921718937</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F30" s="10">
         <v>214.3</v>
@@ -2125,22 +2129,22 @@
         <v>97.2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" s="10">
         <v>2791.6</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D31" s="10">
         <f>B31/2.20462</f>
         <v>1266.2499659805319</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F31" s="10">
         <v>215.4</v>
@@ -2150,23 +2154,23 @@
         <v>97.703912692436802</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="11">
         <f>F32*24.8</f>
         <v>6239.68</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" s="11">
         <f>B32/2.20462</f>
         <v>2830.2746051473728</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F32" s="11">
         <v>251.6</v>
@@ -2176,19 +2180,19 @@
         <v>114.12397601400696</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J32" s="18">
         <f>D32*conversion!B20/(1000*conversion!B4)</f>
         <v>3.0636890225739433</v>
       </c>
       <c r="K32" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -2197,16 +2201,16 @@
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="25">
       <c r="A34" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11">
@@ -2217,22 +2221,22 @@
         <v>7.7065435313115183</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" s="11">
         <v>5771</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D35" s="11">
         <f>B35/2.20462</f>
         <v>2617.6846803530771</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F35" s="11">
         <v>91.9</v>
@@ -2242,22 +2246,22 @@
         <v>41.685188377135297</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B36" s="11">
         <v>6160</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D36" s="11">
         <f>B36/2.20462</f>
         <v>2794.1323221235407</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F36" s="11">
         <v>189.54</v>
@@ -2267,23 +2271,23 @@
         <v>85.974000054431158</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="15" thickBot="1">
       <c r="A37" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B37" s="14">
         <f>F37*4.4</f>
         <v>924.00000000000011</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D37" s="11">
         <f>B37/2.20462</f>
         <v>419.11984831853118</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F37" s="15">
         <v>210</v>
@@ -2293,9 +2297,9 @@
         <v>95.254510981484344</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="13.5" customHeight="1">
       <c r="A38" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38" s="25"/>
       <c r="C38" s="25"/>
@@ -2304,9 +2308,9 @@
       <c r="F38" s="25"/>
       <c r="G38" s="25"/>
     </row>
-    <row r="39" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="11.25" customHeight="1">
       <c r="A39" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
@@ -2316,9 +2320,9 @@
       <c r="G39" s="26"/>
       <c r="K39" s="23"/>
     </row>
-    <row r="40" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="12.75" customHeight="1">
       <c r="A40" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B40" s="26"/>
       <c r="C40" s="26"/>
@@ -2327,7 +2331,7 @@
       <c r="F40" s="26"/>
       <c r="G40" s="26"/>
     </row>
-    <row r="41" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="24" customHeight="1">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2336,7 +2340,7 @@
       <c r="F41" s="27"/>
       <c r="G41" s="27"/>
     </row>
-    <row r="42" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="12" customHeight="1">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2345,9 +2349,9 @@
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -2384,82 +2388,82 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1">
         <v>1055870</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2">
         <f>10^6</f>
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3">
         <f>10^9</f>
         <v>1000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4">
         <v>0.90718399999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5">
         <v>3.6640000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
         <v>29307600000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7">
         <v>3.7854099999999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B12">
         <f>(800+970)/2</f>
@@ -2470,12 +2474,12 @@
         <v>3.35008785</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B13">
         <f>(800+860)/2</f>
@@ -2486,12 +2490,12 @@
         <v>3.1418903</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14">
         <f>(710+790)/2</f>
@@ -2502,28 +2506,28 @@
         <v>2.8390575</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="B15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2532,16 +2536,15 @@
         <v>0.98199999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
       <c r="B21">
-        <f>0.918</f>
-        <v>0.91800000000000004</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.98499999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -2550,7 +2553,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -2558,7 +2561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Update CO2 estimates with liquid biofuel fraction, oxidation fraction options, comparisons to cdiac.
</commit_message>
<xml_diff>
--- a/input/default-emissions-data/CO2_base_EF.xlsx
+++ b/input/default-emissions-data/CO2_base_EF.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="25600" windowHeight="13120" tabRatio="500"/>
+    <workbookView xWindow="13740" yWindow="620" windowWidth="16020" windowHeight="14180" tabRatio="881" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="main" sheetId="1" r:id="rId1"/>
-    <sheet name="CDIAC" sheetId="2" r:id="rId2"/>
-    <sheet name="EIA" sheetId="4" r:id="rId3"/>
-    <sheet name="conversion" sheetId="5" r:id="rId4"/>
+    <sheet name="CDIAC" sheetId="2" r:id="rId1"/>
+    <sheet name="EIA" sheetId="4" r:id="rId2"/>
+    <sheet name="conversion" sheetId="5" r:id="rId3"/>
+    <sheet name="Emission_Coefficient" sheetId="6" r:id="rId4"/>
+    <sheet name="Fraction_Oxidized" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="111">
   <si>
     <t>cdiac_fuel</t>
   </si>
@@ -51,9 +52,6 @@
     <t>gas_flaring</t>
   </si>
   <si>
-    <t>ceds_fuel</t>
-  </si>
-  <si>
     <t>src</t>
   </si>
   <si>
@@ -264,9 +262,6 @@
     <t>light_oil</t>
   </si>
   <si>
-    <t>diesel_oil (aviation)</t>
-  </si>
-  <si>
     <t>diesel</t>
   </si>
   <si>
@@ -306,12 +301,6 @@
     <t>kg/gallon</t>
   </si>
   <si>
-    <t>CDIAC</t>
-  </si>
-  <si>
-    <t>EIA</t>
-  </si>
-  <si>
     <t>Fraction oxidized</t>
   </si>
   <si>
@@ -319,6 +308,54 @@
   </si>
   <si>
     <t>Source: http://cdiac.ornl.gov/epubs/ndp/ndp030/tables/table4.htm</t>
+  </si>
+  <si>
+    <t>iso</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t>fuel</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Emission_Coefficient</t>
+  </si>
+  <si>
+    <t>emission_coefficent</t>
+  </si>
+  <si>
+    <t>1A3aii_Domestic-aviation</t>
+  </si>
+  <si>
+    <t>1A3ai_International-aviation</t>
+  </si>
+  <si>
+    <t>1A3di_International-shipping</t>
+  </si>
+  <si>
+    <t>1A3dii_Domestic-navigation</t>
+  </si>
+  <si>
+    <t>Fraction_Oxidized</t>
+  </si>
+  <si>
+    <t>hard_coal</t>
+  </si>
+  <si>
+    <t>brown_coal</t>
+  </si>
+  <si>
+    <t>natural_gas</t>
+  </si>
+  <si>
+    <t>chn</t>
+  </si>
+  <si>
+    <t>discussed in data and assumptions supplement</t>
   </si>
 </sst>
 </file>
@@ -328,7 +365,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -405,11 +442,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -420,16 +452,41 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -519,8 +576,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="54">
+  <cellStyleXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -596,8 +668,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -641,18 +741,19 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="29" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="24" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="24" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="24" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="24" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="2" xfId="25" applyNumberFormat="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="0" xfId="25" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="11" fillId="0" borderId="2" xfId="25" applyNumberFormat="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="11" fillId="0" borderId="0" xfId="25" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="2" xfId="25" applyNumberFormat="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="24" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="54"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="28" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -675,7 +776,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="54">
+  <cellStyles count="82">
     <cellStyle name="Body: normal cell" xfId="25"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -707,6 +808,33 @@
     <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
     <cellStyle name="Font: Calibri, 9pt regular" xfId="30"/>
     <cellStyle name="Footnotes: all except top row" xfId="31"/>
     <cellStyle name="Footnotes: top row" xfId="28"/>
@@ -726,6 +854,7 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="24"/>
+    <cellStyle name="Output" xfId="54" builtinId="21"/>
     <cellStyle name="Parent row" xfId="26"/>
     <cellStyle name="Section Break" xfId="33"/>
     <cellStyle name="Section Break: parent row" xfId="34"/>
@@ -1063,193 +1192,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="3" max="3" width="12" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="B2" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <f>CDIAC!E2</f>
+      <c r="B2">
+        <v>0.72409999999999997</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1">
+        <f>B2*conversion!B5/conversion!B6</f>
         <v>9.0526088796080198E-11</v>
       </c>
-      <c r="D2" s="1" t="str">
-        <f>CDIAC!F2</f>
-        <v>kt CO2/kJ</v>
-      </c>
-      <c r="E2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="B3" t="s">
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="1">
+        <f>E2/conversion!B20</f>
+        <v>9.2185426472586756E-11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <f>CDIAC!E3</f>
+      <c r="B3">
+        <f>0.85*conversion!B21</f>
+        <v>0.83724999999999994</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <f>B3*conversion!B5</f>
         <v>3.0676839999999999</v>
       </c>
-      <c r="D3" s="1" t="str">
-        <f>CDIAC!F3</f>
-        <v>kt CO2/kt</v>
-      </c>
-      <c r="E3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4" t="s">
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3">
+        <f>E3/conversion!B21</f>
+        <v>3.1143999999999998</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
-        <f>CDIAC!E4</f>
+      <c r="B4">
+        <f>0.0137*conversion!B22</f>
+        <v>1.3426E-2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <f>B4*conversion!B5</f>
         <v>4.9192864000000003E-2</v>
       </c>
-      <c r="D4" s="1" t="str">
-        <f>CDIAC!F4</f>
-        <v>kt CO2/TJ</v>
-      </c>
-      <c r="E4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="B5" t="s">
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4">
+        <f>E4/conversion!B22</f>
+        <v>5.0196800000000007E-2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
-        <f>CDIAC!E5</f>
+      <c r="B5">
+        <f>0.855*conversion!B23</f>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <f>B5*conversion!B5</f>
         <v>3.1327199999999999</v>
       </c>
-      <c r="D5" s="1" t="str">
-        <f>CDIAC!F5</f>
-        <v>kt CO2/kt</v>
-      </c>
-      <c r="E5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" t="s">
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5">
+        <f>E5</f>
+        <v>3.1327199999999999</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
-        <f>CDIAC!E6</f>
+      <c r="B6">
+        <f>13.454*conversion!B24</f>
+        <v>13.454000000000001</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <f>B6*conversion!B5/1000</f>
         <v>4.9295456000000001E-2</v>
       </c>
-      <c r="D6" s="1" t="str">
-        <f>CDIAC!F6</f>
-        <v>kt CO2/TJ</v>
-      </c>
-      <c r="E6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <f>EIA!J32</f>
-        <v>3.0636890225739433</v>
-      </c>
-      <c r="D7" t="str">
-        <f>EIA!K32</f>
-        <v>kt CO2/kt</v>
-      </c>
-      <c r="E7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8">
-        <f>EIA!J19</f>
-        <v>4.3210700017102557</v>
-      </c>
-      <c r="D8" t="str">
-        <f>EIA!K19</f>
-        <v>kt CO2/kt</v>
-      </c>
-      <c r="E8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9">
-        <f>EIA!J8</f>
-        <v>3.1853670873830175</v>
-      </c>
-      <c r="D9" t="str">
-        <f>EIA!K8</f>
-        <v>kt CO2/kt</v>
-      </c>
-      <c r="E9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10">
-        <f>EIA!J12</f>
-        <v>3.084497129615889</v>
-      </c>
-      <c r="D10" t="str">
-        <f>EIA!K12</f>
-        <v>kt CO2/kt</v>
-      </c>
-      <c r="E10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11">
-        <f>EIA!J15</f>
-        <v>3.0461949575680598</v>
-      </c>
-      <c r="D11" t="str">
-        <f>EIA!K15</f>
-        <v>kt CO2/kt</v>
-      </c>
-      <c r="E11" t="s">
-        <v>95</v>
-      </c>
+      <c r="F6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6">
+        <f>E6</f>
+        <v>4.9295456000000001E-2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="D9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1263,162 +1367,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>0.72409999999999997</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1">
-        <f>B2*conversion!B5/conversion!B6</f>
-        <v>9.0526088796080198E-11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <f>0.85*conversion!B21</f>
-        <v>0.83724999999999994</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3">
-        <f>B3*conversion!B5</f>
-        <v>3.0676839999999999</v>
-      </c>
-      <c r="F3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <f>0.0137*conversion!B22</f>
-        <v>1.3426E-2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4">
-        <f>B4*conversion!B5</f>
-        <v>4.9192864000000003E-2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <f>0.855*conversion!B23</f>
-        <v>0.85499999999999998</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5">
-        <f>B5*conversion!B5</f>
-        <v>3.1327199999999999</v>
-      </c>
-      <c r="F5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <f>13.454*conversion!B24</f>
-        <v>13.454000000000001</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6">
-        <f>B6*conversion!B5/1000</f>
-        <v>4.9295456000000001E-2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="D9" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1436,79 +1388,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A1" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="A1" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="27.75" customHeight="1" thickBot="1">
       <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" thickTop="1">
+      <c r="A4" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A4" s="29" t="s">
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="J4" s="25"/>
+    </row>
+    <row r="5" spans="1:11" ht="15">
+      <c r="A5" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="10" t="s">
-        <v>28</v>
       </c>
       <c r="B5" s="10">
         <v>12.7</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="10">
         <f t="shared" ref="D5:D13" si="0">B5/2.20462</f>
         <v>5.7606299498326248</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="10">
         <v>139.04859867504859</v>
@@ -1517,23 +1473,24 @@
         <f>(F5/2.20462)</f>
         <v>63.071458425963932</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="J5" s="25"/>
+    </row>
+    <row r="6" spans="1:11" ht="15">
       <c r="A6" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="10">
         <v>14.8</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="10">
         <f t="shared" si="0"/>
         <v>6.7131750596474689</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="10">
         <v>143.19829002512873</v>
@@ -1542,23 +1499,24 @@
         <f t="shared" ref="G6:G13" si="1">(F6/2.20462)</f>
         <v>64.953728998706694</v>
       </c>
+      <c r="J6" s="25"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1">
       <c r="A7" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="10">
         <v>13.7</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="10">
         <f t="shared" si="0"/>
         <v>6.214222859268264</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="10">
         <v>141.12344435008868</v>
@@ -1567,23 +1525,24 @@
         <f t="shared" si="1"/>
         <v>64.012593712335317</v>
       </c>
+      <c r="J7" s="25"/>
     </row>
     <row r="8" spans="1:11" ht="26.25" customHeight="1">
-      <c r="A8" s="21" t="s">
-        <v>32</v>
+      <c r="A8" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="B8" s="10">
         <v>22.4</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="10">
         <f t="shared" si="0"/>
         <v>10.160481171358329</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="10">
         <v>161.30000000000001</v>
@@ -1593,32 +1552,32 @@
         <v>73.164536291968702</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="J8" s="18">
-        <f>D8*conversion!B21/conversion!C13</f>
-        <v>3.1853670873830175</v>
+        <v>79</v>
+      </c>
+      <c r="J8" s="25">
+        <f>D8/conversion!C13</f>
+        <v>3.2338752156172763</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15">
       <c r="A9" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="10">
         <v>21.5</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="10">
         <f t="shared" si="0"/>
         <v>9.7522475528662547</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="10">
         <v>159.4</v>
@@ -1627,23 +1586,24 @@
         <f t="shared" si="1"/>
         <v>72.302709764040983</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="J9" s="25"/>
+    </row>
+    <row r="10" spans="1:11" ht="15">
       <c r="A10" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="10">
         <v>4631.5</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="10">
         <f t="shared" si="0"/>
         <v>2100.8155600511654</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="10">
         <v>210.2</v>
@@ -1652,23 +1612,24 @@
         <f t="shared" si="1"/>
         <v>95.345229563371475</v>
       </c>
+      <c r="J10" s="25"/>
     </row>
     <row r="11" spans="1:11" ht="25">
       <c r="A11" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="10">
         <v>117.1</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="10">
         <f t="shared" si="0"/>
         <v>53.115729694913412</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" s="10">
         <v>117</v>
@@ -1677,23 +1638,24 @@
         <f t="shared" si="1"/>
         <v>53.070370403969847</v>
       </c>
+      <c r="J11" s="25"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
-      <c r="A12" s="21" t="s">
-        <v>38</v>
+      <c r="A12" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="B12" s="10">
         <v>19.600000000000001</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="10">
         <f t="shared" si="0"/>
         <v>8.89042102493854</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" s="10">
         <v>157.19999999999999</v>
@@ -1702,32 +1664,32 @@
         <v>71.3</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J12" s="18">
-        <f>D12*conversion!B21/conversion!C14</f>
-        <v>3.084497129615889</v>
+        <v>83</v>
+      </c>
+      <c r="J12" s="25">
+        <f>D12/conversion!C14</f>
+        <v>3.1314691671227299</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="25">
       <c r="A13" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="10">
         <v>26</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="10">
         <f t="shared" si="0"/>
         <v>11.793415645326633</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="10">
         <v>173.7</v>
@@ -1736,34 +1698,36 @@
         <f t="shared" si="1"/>
         <v>78.789088368970624</v>
       </c>
+      <c r="J13" s="25"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="J14" s="25"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1">
+      <c r="A15" s="19" t="s">
         <v>40</v>
-      </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-    </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1">
-      <c r="A15" s="21" t="s">
-        <v>41</v>
       </c>
       <c r="B15" s="10">
         <v>21.1</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="10">
         <f>B15/2.20462</f>
         <v>9.5708103890919993</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="10">
         <v>156.30000000000001</v>
@@ -1773,32 +1737,32 @@
         <v>70.896571744790492</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J15" s="18">
-        <f>D15*conversion!B23/conversion!C13</f>
+        <v>80</v>
+      </c>
+      <c r="J15" s="25">
+        <f>D15/conversion!C13</f>
         <v>3.0461949575680598</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="10">
         <v>18.399999999999999</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="10">
         <f>B16/2.20462</f>
         <v>8.3461095336157705</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" s="10">
         <v>152.6</v>
@@ -1806,34 +1770,36 @@
       <c r="G16" s="10">
         <v>69.2</v>
       </c>
+      <c r="J16" s="25"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A17" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
+      <c r="A17" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="J17" s="25"/>
     </row>
     <row r="18" spans="1:11" ht="22.5" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="10">
         <v>120.7</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="10">
         <f>B18/2.20462</f>
         <v>54.748664168881717</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="10">
         <v>120.6</v>
@@ -1842,23 +1808,24 @@
         <f>(F18/2.20462)</f>
         <v>54.703304877938152</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="21" t="s">
-        <v>45</v>
+      <c r="J18" s="25"/>
+    </row>
+    <row r="19" spans="1:11" ht="15">
+      <c r="A19" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="B19" s="10">
         <v>32.4</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" s="10">
         <f>B19/2.20462</f>
         <v>14.696410265714727</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F19" s="10">
         <v>225.1</v>
@@ -1868,33 +1835,33 @@
         <v>102.10376391396251</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="J19" s="18">
-        <f>D19*conversion!B21/conversion!C12</f>
-        <v>4.3210700017102557</v>
-      </c>
-      <c r="K19" s="23" t="s">
-        <v>75</v>
+        <v>82</v>
+      </c>
+      <c r="J19" s="25">
+        <f>D19/conversion!C12</f>
+        <v>4.3868730981830009</v>
+      </c>
+      <c r="K19" s="21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="25">
       <c r="A20" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="10">
         <f>F20*5.796/42</f>
         <v>22.093800000000002</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="10">
         <f>B20/2.20462</f>
         <v>10.021591022489138</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F20" s="10">
         <v>160.1</v>
@@ -1903,35 +1870,37 @@
         <f>(F20/2.20462)</f>
         <v>72.620224800645914</v>
       </c>
+      <c r="J20" s="25"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="J21" s="25"/>
+    </row>
+    <row r="22" spans="1:11" ht="15">
+      <c r="A22" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="10" t="s">
-        <v>48</v>
       </c>
       <c r="B22" s="10">
         <f>F22*6.636/42</f>
         <v>26.3386</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22" s="10">
         <f>B22/2.20462</f>
         <v>11.94700220446154</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F22" s="10">
         <v>166.7</v>
@@ -1940,24 +1909,25 @@
         <f>(F22/2.20462)</f>
         <v>75.613938002921145</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="24" t="s">
-        <v>49</v>
+      <c r="J22" s="25"/>
+    </row>
+    <row r="23" spans="1:11" ht="15">
+      <c r="A23" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="B23" s="10">
         <f>F23*6.065/42</f>
         <v>23.624619047619049</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" s="10">
         <f>B23/2.20462</f>
         <v>10.715959688118158</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F23" s="10">
         <v>163.6</v>
@@ -1966,25 +1936,26 @@
         <f>(F23/2.20462)</f>
         <v>74.207799983670654</v>
       </c>
-      <c r="K23" s="23"/>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="J23" s="25"/>
+      <c r="K23" s="21"/>
+    </row>
+    <row r="24" spans="1:11" ht="15">
       <c r="A24" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="10">
         <f>F24*6.636/42</f>
         <v>24.742799999999999</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D24" s="10">
         <f>B24/2.20462</f>
         <v>11.223158639584147</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" s="10">
         <v>156.6</v>
@@ -1993,24 +1964,25 @@
         <f>(F24/2.20462)</f>
         <v>71.032649617621175</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="J24" s="25"/>
+    </row>
+    <row r="25" spans="1:11" ht="15">
       <c r="A25" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" s="10">
         <f>F25*5.248/42</f>
         <v>20.054857142857145</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D25" s="10">
         <f>B25/2.20462</f>
         <v>9.0967409997446946</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F25" s="10">
         <v>160.5</v>
@@ -2019,24 +1991,25 @@
         <f>(F25/2.20462)</f>
         <v>72.801661964420177</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="J25" s="25"/>
+    </row>
+    <row r="26" spans="1:11" ht="15">
       <c r="A26" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="10">
         <f>F26*5.537/42</f>
         <v>21.106516666666668</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D26" s="10">
         <f>B26/2.20462</f>
         <v>9.5737663028851543</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F26" s="10">
         <v>160.1</v>
@@ -2045,34 +2018,36 @@
         <f>(F26/2.20462)</f>
         <v>72.620224800645914</v>
       </c>
+      <c r="J26" s="25"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="J27" s="25"/>
+    </row>
+    <row r="28" spans="1:11" ht="15">
+      <c r="A28" s="10" t="s">
         <v>53</v>
-      </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="10" t="s">
-        <v>54</v>
       </c>
       <c r="B28" s="10">
         <v>5685</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="10">
         <f>B28/2.20462</f>
         <v>2578.675690141612</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F28" s="10">
         <v>228.6</v>
@@ -2080,23 +2055,24 @@
       <c r="G28" s="10">
         <v>103.7</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="J28" s="25"/>
+    </row>
+    <row r="29" spans="1:11" ht="15">
       <c r="A29" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="10">
         <v>4931.3</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" s="10">
         <f>B29/2.20462</f>
         <v>2236.8027142999704</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F29" s="10">
         <v>205.7</v>
@@ -2104,23 +2080,24 @@
       <c r="G29" s="10">
         <v>93.3</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="J29" s="25"/>
+    </row>
+    <row r="30" spans="1:11" ht="15">
       <c r="A30" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" s="10">
         <v>3715.9</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" s="10">
         <f>B30/2.20462</f>
         <v>1685.5058921718937</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F30" s="10">
         <v>214.3</v>
@@ -2128,23 +2105,24 @@
       <c r="G30" s="10">
         <v>97.2</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="J30" s="25"/>
+    </row>
+    <row r="31" spans="1:11" ht="15">
       <c r="A31" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" s="10">
         <v>2791.6</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" s="10">
         <f>B31/2.20462</f>
         <v>1266.2499659805319</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F31" s="10">
         <v>215.4</v>
@@ -2153,24 +2131,25 @@
         <f>(F31/2.20462)</f>
         <v>97.703912692436802</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="22" t="s">
-        <v>58</v>
+      <c r="J31" s="25"/>
+    </row>
+    <row r="32" spans="1:11" ht="15">
+      <c r="A32" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="B32" s="11">
         <f>F32*24.8</f>
         <v>6239.68</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="11">
         <f>B32/2.20462</f>
         <v>2830.2746051473728</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F32" s="11">
         <v>251.6</v>
@@ -2180,19 +2159,19 @@
         <v>114.12397601400696</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J32" s="18">
-        <f>D32*conversion!B20/(1000*conversion!B4)</f>
-        <v>3.0636890225739433</v>
+        <v>81</v>
+      </c>
+      <c r="J32" s="25">
+        <f>D32/(1000*conversion!B4)</f>
+        <v>3.1198462551669484</v>
       </c>
       <c r="K32" s="18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15">
       <c r="A33" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -2200,17 +2179,18 @@
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
+      <c r="J33" s="25"/>
     </row>
     <row r="34" spans="1:11" ht="25">
       <c r="A34" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="13" t="s">
         <v>60</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>61</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11">
@@ -2223,20 +2203,20 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B35" s="11">
         <v>5771</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D35" s="11">
         <f>B35/2.20462</f>
         <v>2617.6846803530771</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F35" s="11">
         <v>91.9</v>
@@ -2248,20 +2228,20 @@
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" s="11">
         <v>6160</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="11">
         <f>B36/2.20462</f>
         <v>2794.1323221235407</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F36" s="11">
         <v>189.54</v>
@@ -2273,21 +2253,21 @@
     </row>
     <row r="37" spans="1:11" ht="15" thickBot="1">
       <c r="A37" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" s="14">
         <f>F37*4.4</f>
         <v>924.00000000000011</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D37" s="11">
         <f>B37/2.20462</f>
         <v>419.11984831853118</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F37" s="15">
         <v>210</v>
@@ -2298,47 +2278,47 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+    </row>
+    <row r="39" spans="1:11" ht="11.25" customHeight="1">
+      <c r="A39" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-    </row>
-    <row r="39" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A39" s="26" t="s">
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="K39" s="21"/>
+    </row>
+    <row r="40" spans="1:11" ht="12.75" customHeight="1">
+      <c r="A40" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="K39" s="23"/>
-    </row>
-    <row r="40" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A40" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
     </row>
     <row r="41" spans="1:11" ht="24" customHeight="1">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
     </row>
     <row r="42" spans="1:11" ht="12" customHeight="1">
       <c r="A42" s="4"/>
@@ -2351,7 +2331,7 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -2375,6 +2355,204 @@
     <hyperlink ref="A43" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1">
+        <v>1055870</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2">
+        <f>10^6</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3">
+        <f>10^9</f>
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4">
+        <v>0.90718399999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5">
+        <v>3.6640000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
+        <v>29307600000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7">
+        <v>3.7854099999999999E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12">
+        <f>(800+970)/2</f>
+        <v>885</v>
+      </c>
+      <c r="C12">
+        <f>B12*$B$7</f>
+        <v>3.35008785</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13">
+        <f>(800+860)/2</f>
+        <v>830</v>
+      </c>
+      <c r="C13">
+        <f>B13*$B$7</f>
+        <v>3.1418903</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14">
+        <f>(710+790)/2</f>
+        <v>750</v>
+      </c>
+      <c r="C14">
+        <f>B14*$B$7</f>
+        <v>2.8390575</v>
+      </c>
+      <c r="D14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <f>0.982</f>
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>0.98499999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <f>0.98</f>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2385,192 +2563,491 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1">
-        <v>1055870</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2">
-        <f>10^6</f>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CDIAC!F2</f>
+        <v>kt CO2/kJ</v>
+      </c>
+      <c r="E2" s="1">
+        <f>CDIAC!G2</f>
+        <v>9.2185426472586756E-11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3">
-        <f>10^9</f>
-        <v>1000000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="str">
+        <f>CDIAC!F2</f>
+        <v>kt CO2/kJ</v>
+      </c>
+      <c r="E3" s="1">
+        <f>CDIAC!G2</f>
+        <v>9.2185426472586756E-11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4">
-        <v>0.90718399999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f>CDIAC!F4</f>
+        <v>kt CO2/TJ</v>
+      </c>
+      <c r="E4">
+        <f>CDIAC!G4</f>
+        <v>5.0196800000000007E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5">
-        <v>3.6640000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f>CDIAC!F5</f>
+        <v>kt CO2/kt</v>
+      </c>
+      <c r="E5">
+        <f>CDIAC!G5</f>
+        <v>3.1327199999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1">
-        <v>29307600000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f>CDIAC!F6</f>
+        <v>kt CO2/TJ</v>
+      </c>
+      <c r="E6">
+        <f>CDIAC!G6</f>
+        <v>4.9295456000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B7">
-        <v>3.7854099999999999E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f>EIA!K8</f>
+        <v>kt CO2/kt</v>
+      </c>
+      <c r="E7">
+        <f>EIA!J12</f>
+        <v>3.1314691671227299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8">
+        <f>EIA!J8</f>
+        <v>3.2338752156172763</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" t="str">
+        <f>EIA!K19</f>
+        <v>kt CO2/kt</v>
+      </c>
+      <c r="E9">
+        <f>EIA!J19</f>
+        <v>4.3868730981830009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="str">
+        <f>EIA!K32</f>
+        <v>kt CO2/kt</v>
+      </c>
+      <c r="E10">
+        <f>EIA!J32</f>
+        <v>3.1198462551669484</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>98</v>
+      </c>
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="24" t="str">
+        <f>EIA!K15</f>
+        <v>kt CO2/kt</v>
+      </c>
+      <c r="E11" s="24">
+        <f>EIA!J$8</f>
+        <v>3.2338752156172763</v>
+      </c>
+      <c r="F11" s="24"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12">
-        <f>(800+970)/2</f>
-        <v>885</v>
-      </c>
-      <c r="C12">
-        <f>B12*$B$7</f>
-        <v>3.35008785</v>
-      </c>
-      <c r="D12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="D12" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="24">
+        <f>EIA!J$8</f>
+        <v>3.2338752156172763</v>
+      </c>
+      <c r="F12" s="24"/>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13">
-        <f>(800+860)/2</f>
-        <v>830</v>
-      </c>
-      <c r="C13">
-        <f>B13*$B$7</f>
-        <v>3.1418903</v>
-      </c>
-      <c r="D13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>98</v>
+      </c>
+      <c r="B13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="24">
+        <f>CDIAC!G5</f>
+        <v>3.1327199999999999</v>
+      </c>
+      <c r="F13" s="24"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14">
-        <f>(710+790)/2</f>
-        <v>750</v>
-      </c>
-      <c r="C14">
-        <f>B14*$B$7</f>
-        <v>2.8390575</v>
-      </c>
-      <c r="D14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="B15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20">
-        <f>0.982</f>
-        <v>0.98199999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21">
-        <v>0.98499999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22">
-        <f>0.98</f>
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="24">
+        <f>CDIAC!G5</f>
+        <v>3.1327199999999999</v>
+      </c>
+      <c r="F14" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="23">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="23">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="23">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="23">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="E5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="23">
+        <v>0.98499999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="23">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.98</v>
+      </c>
+      <c r="E8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="23">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="23">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="23">
+        <v>0.96</v>
+      </c>
+      <c r="E11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="23">
+        <v>0.96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
CO2 oxidation fraction and biofuel correction. Same as master branch
</commit_message>
<xml_diff>
--- a/input/default-emissions-data/CO2_base_EF.xlsx
+++ b/input/default-emissions-data/CO2_base_EF.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6345" yWindow="0" windowWidth="19320" windowHeight="13935" tabRatio="500"/>
+    <workbookView xWindow="13740" yWindow="620" windowWidth="16020" windowHeight="14180" tabRatio="881" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="main" sheetId="1" r:id="rId1"/>
-    <sheet name="CDIAC" sheetId="2" r:id="rId2"/>
-    <sheet name="EIA" sheetId="4" r:id="rId3"/>
-    <sheet name="conversion" sheetId="5" r:id="rId4"/>
+    <sheet name="CDIAC" sheetId="2" r:id="rId1"/>
+    <sheet name="EIA" sheetId="4" r:id="rId2"/>
+    <sheet name="conversion" sheetId="5" r:id="rId3"/>
+    <sheet name="Emission_Coefficient" sheetId="6" r:id="rId4"/>
+    <sheet name="Fraction_Oxidized" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="111">
   <si>
     <t>cdiac_fuel</t>
   </si>
@@ -51,18 +52,12 @@
     <t>gas_flaring</t>
   </si>
   <si>
-    <t>ceds_fuel</t>
-  </si>
-  <si>
     <t>src</t>
   </si>
   <si>
     <t>coal_coke</t>
   </si>
   <si>
-    <t>http://cdiac.ornl.gov/pns/convert.html</t>
-  </si>
-  <si>
     <t>https://www.eia.gov/environment/emissions/co2_vol_mass.cfm</t>
   </si>
   <si>
@@ -267,9 +262,6 @@
     <t>light_oil</t>
   </si>
   <si>
-    <t>diesel_oil (aviation)</t>
-  </si>
-  <si>
     <t>diesel</t>
   </si>
   <si>
@@ -309,19 +301,61 @@
     <t>kg/gallon</t>
   </si>
   <si>
-    <t>CDIAC</t>
-  </si>
-  <si>
-    <t>EIA</t>
-  </si>
-  <si>
     <t>Fraction oxidized</t>
   </si>
   <si>
-    <t>Source: http://cdiac.ornl.gov/pns/convert.html; http://cdiac.ornl.gov/epubs/ndp/ndp030/tables/table4.htm</t>
-  </si>
-  <si>
     <t>personal correspondence, also http://cdiac.ornl.gov/pns/convert.html</t>
+  </si>
+  <si>
+    <t>Source: http://cdiac.ornl.gov/epubs/ndp/ndp030/tables/table4.htm</t>
+  </si>
+  <si>
+    <t>iso</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t>fuel</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Emission_Coefficient</t>
+  </si>
+  <si>
+    <t>emission_coefficent</t>
+  </si>
+  <si>
+    <t>1A3aii_Domestic-aviation</t>
+  </si>
+  <si>
+    <t>1A3ai_International-aviation</t>
+  </si>
+  <si>
+    <t>1A3di_International-shipping</t>
+  </si>
+  <si>
+    <t>1A3dii_Domestic-navigation</t>
+  </si>
+  <si>
+    <t>Fraction_Oxidized</t>
+  </si>
+  <si>
+    <t>hard_coal</t>
+  </si>
+  <si>
+    <t>brown_coal</t>
+  </si>
+  <si>
+    <t>natural_gas</t>
+  </si>
+  <si>
+    <t>chn</t>
+  </si>
+  <si>
+    <t>discussed in data and assumptions supplement</t>
   </si>
 </sst>
 </file>
@@ -331,7 +365,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -408,11 +442,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -423,16 +452,41 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -522,8 +576,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="52">
+  <cellStyleXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -597,8 +666,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -642,18 +741,19 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="29" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="24" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="24" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="24" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="24" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="2" xfId="25" applyNumberFormat="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="0" borderId="0" xfId="25" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="11" fillId="0" borderId="2" xfId="25" applyNumberFormat="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="11" fillId="0" borderId="0" xfId="25" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="2" xfId="25" applyNumberFormat="1" applyFont="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="24" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="54"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="28" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -676,7 +776,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="52">
+  <cellStyles count="82">
     <cellStyle name="Body: normal cell" xfId="25"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -706,6 +806,35 @@
     <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
     <cellStyle name="Font: Calibri, 9pt regular" xfId="30"/>
     <cellStyle name="Footnotes: all except top row" xfId="31"/>
     <cellStyle name="Footnotes: top row" xfId="28"/>
@@ -725,6 +854,7 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="24"/>
+    <cellStyle name="Output" xfId="54" builtinId="21"/>
     <cellStyle name="Parent row" xfId="26"/>
     <cellStyle name="Section Break" xfId="33"/>
     <cellStyle name="Section Break: parent row" xfId="34"/>
@@ -1062,193 +1192,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="12" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <f>CDIAC!E2</f>
+      <c r="B2">
+        <v>0.72409999999999997</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1">
+        <f>B2*conversion!B5/conversion!B6</f>
         <v>9.0526088796080198E-11</v>
       </c>
-      <c r="D2" s="1" t="str">
-        <f>CDIAC!F2</f>
-        <v>kt CO2/kJ</v>
-      </c>
-      <c r="E2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="1">
+        <f>E2/conversion!B20</f>
+        <v>9.2185426472586756E-11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <f>CDIAC!E3</f>
-        <v>3.0676840000000003</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f>CDIAC!F3</f>
-        <v>kt CO2/kt</v>
-      </c>
-      <c r="E3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B3">
+        <f>0.85*conversion!B21</f>
+        <v>0.83724999999999994</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <f>B3*conversion!B5</f>
+        <v>3.0676839999999999</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3">
+        <f>E3/conversion!B21</f>
+        <v>3.1143999999999998</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
-        <f>CDIAC!E4</f>
+      <c r="B4">
+        <f>0.0137*conversion!B22</f>
+        <v>1.3426E-2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <f>B4*conversion!B5</f>
         <v>4.9192864000000003E-2</v>
       </c>
-      <c r="D4" s="1" t="str">
-        <f>CDIAC!F4</f>
-        <v>kt CO2/TJ</v>
-      </c>
-      <c r="E4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4">
+        <f>E4/conversion!B22</f>
+        <v>5.0196800000000007E-2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
-        <f>CDIAC!E5</f>
+      <c r="B5">
+        <f>0.855*conversion!B23</f>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <f>B5*conversion!B5</f>
         <v>3.1327199999999999</v>
       </c>
-      <c r="D5" s="1" t="str">
-        <f>CDIAC!F5</f>
-        <v>kt CO2/kt</v>
-      </c>
-      <c r="E5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5">
+        <f>E5</f>
+        <v>3.1327199999999999</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
-        <f>CDIAC!E6</f>
+      <c r="B6">
+        <f>13.454*conversion!B24</f>
+        <v>13.454000000000001</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <f>B6*conversion!B5/1000</f>
         <v>4.9295456000000001E-2</v>
       </c>
-      <c r="D6" s="1" t="str">
-        <f>CDIAC!F6</f>
-        <v>kt CO2/TJ</v>
-      </c>
-      <c r="E6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <f>EIA!J32</f>
-        <v>3.0636890225739433</v>
-      </c>
-      <c r="D7" t="str">
-        <f>EIA!K32</f>
-        <v>kt CO2/kt</v>
-      </c>
-      <c r="E7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8">
-        <f>EIA!J19</f>
-        <v>4.0271495041319945</v>
-      </c>
-      <c r="D8" t="str">
-        <f>EIA!K19</f>
-        <v>kt CO2/kt</v>
-      </c>
-      <c r="E8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9">
-        <f>EIA!J8</f>
-        <v>2.9686974479366599</v>
-      </c>
-      <c r="D9" t="str">
-        <f>EIA!K8</f>
-        <v>kt CO2/kt</v>
-      </c>
-      <c r="E9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10">
-        <f>EIA!J12</f>
-        <v>2.8746886954186661</v>
-      </c>
-      <c r="D10" t="str">
-        <f>EIA!K12</f>
-        <v>kt CO2/kt</v>
-      </c>
-      <c r="E10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11">
-        <f>EIA!J15</f>
-        <v>3.0461949575680598</v>
-      </c>
-      <c r="D11" t="str">
-        <f>EIA!K15</f>
-        <v>kt CO2/kt</v>
-      </c>
-      <c r="E11" t="s">
-        <v>96</v>
-      </c>
+      <c r="F6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6">
+        <f>E6</f>
+        <v>4.9295456000000001E-2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="D9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1262,249 +1367,104 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>0.72409999999999997</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="1">
-        <f>B2*conversion!B5/conversion!B6</f>
-        <v>9.0526088796080198E-11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>0.83725000000000005</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3">
-        <f>B3*conversion!B5</f>
-        <v>3.0676840000000003</v>
-      </c>
-      <c r="F3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1.3426E-2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4">
-        <f>B4*conversion!B5</f>
-        <v>4.9192864000000003E-2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>0.85499999999999998</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5">
-        <f>B5*conversion!B5</f>
-        <v>3.1327199999999999</v>
-      </c>
-      <c r="F5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>13.454000000000001</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <f>B6*conversion!B5/1000</f>
-        <v>4.9295456000000001E-2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19" style="3" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="17" customWidth="1"/>
-    <col min="7" max="7" width="11.625" style="17" customWidth="1"/>
-    <col min="8" max="9" width="8.875" style="3"/>
-    <col min="10" max="11" width="8.875" style="18"/>
-    <col min="12" max="16384" width="8.875" style="3"/>
+    <col min="7" max="7" width="11.6640625" style="17" customWidth="1"/>
+    <col min="8" max="9" width="8.83203125" style="3"/>
+    <col min="10" max="11" width="8.83203125" style="18"/>
+    <col min="12" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-    </row>
-    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="18.75" customHeight="1">
+      <c r="A1" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+    </row>
+    <row r="2" spans="1:11" ht="30" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="27.75" customHeight="1" thickBot="1">
+      <c r="A3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" thickTop="1">
+      <c r="A4" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="J4" s="25"/>
+    </row>
+    <row r="5" spans="1:11" ht="15">
+      <c r="A5" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="B5" s="10">
         <v>12.7</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="10">
         <f t="shared" ref="D5:D13" si="0">B5/2.20462</f>
         <v>5.7606299498326248</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" s="10">
         <v>139.04859867504859</v>
@@ -1513,23 +1473,24 @@
         <f>(F5/2.20462)</f>
         <v>63.071458425963932</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" s="25"/>
+    </row>
+    <row r="6" spans="1:11" ht="15">
       <c r="A6" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="10">
         <v>14.8</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="10">
         <f t="shared" si="0"/>
         <v>6.7131750596474689</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" s="10">
         <v>143.19829002512873</v>
@@ -1538,23 +1499,24 @@
         <f t="shared" ref="G6:G13" si="1">(F6/2.20462)</f>
         <v>64.953728998706694</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="25"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1">
       <c r="A7" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="10">
         <v>13.7</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" s="10">
         <f t="shared" si="0"/>
         <v>6.214222859268264</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7" s="10">
         <v>141.12344435008868</v>
@@ -1563,23 +1525,24 @@
         <f t="shared" si="1"/>
         <v>64.012593712335317</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>33</v>
+      <c r="J7" s="25"/>
+    </row>
+    <row r="8" spans="1:11" ht="26.25" customHeight="1">
+      <c r="A8" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="B8" s="10">
         <v>22.4</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8" s="10">
         <f t="shared" si="0"/>
         <v>10.160481171358329</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F8" s="10">
         <v>161.30000000000001</v>
@@ -1589,32 +1552,32 @@
         <v>73.164536291968702</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J8" s="18">
-        <f>D8*conversion!B21/conversion!C13</f>
-        <v>2.9686974479366599</v>
+        <v>79</v>
+      </c>
+      <c r="J8" s="25">
+        <f>D8/conversion!C13</f>
+        <v>3.2338752156172763</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15">
       <c r="A9" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" s="10">
         <v>21.5</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D9" s="10">
         <f t="shared" si="0"/>
         <v>9.7522475528662547</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F9" s="10">
         <v>159.4</v>
@@ -1623,23 +1586,24 @@
         <f t="shared" si="1"/>
         <v>72.302709764040983</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" s="25"/>
+    </row>
+    <row r="10" spans="1:11" ht="15">
       <c r="A10" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="10">
         <v>4631.5</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="10">
         <f t="shared" si="0"/>
         <v>2100.8155600511654</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F10" s="10">
         <v>210.2</v>
@@ -1648,23 +1612,24 @@
         <f t="shared" si="1"/>
         <v>95.345229563371475</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="J10" s="25"/>
+    </row>
+    <row r="11" spans="1:11" ht="25">
       <c r="A11" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" s="10">
         <v>117.1</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" s="10">
         <f t="shared" si="0"/>
         <v>53.115729694913412</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F11" s="10">
         <v>117</v>
@@ -1673,23 +1638,24 @@
         <f t="shared" si="1"/>
         <v>53.070370403969847</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
-        <v>39</v>
+      <c r="J11" s="25"/>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1">
+      <c r="A12" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="B12" s="10">
         <v>19.600000000000001</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12" s="10">
         <f t="shared" si="0"/>
         <v>8.89042102493854</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F12" s="10">
         <v>157.19999999999999</v>
@@ -1698,32 +1664,32 @@
         <v>71.3</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J12" s="18">
-        <f>D12*conversion!B21/conversion!C14</f>
-        <v>2.8746886954186661</v>
+        <v>83</v>
+      </c>
+      <c r="J12" s="25">
+        <f>D12/conversion!C14</f>
+        <v>3.1314691671227299</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="25">
       <c r="A13" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" s="10">
         <v>26</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" s="10">
         <f t="shared" si="0"/>
         <v>11.793415645326633</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F13" s="10">
         <v>173.7</v>
@@ -1732,34 +1698,36 @@
         <f t="shared" si="1"/>
         <v>78.789088368970624</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-    </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>42</v>
+      <c r="J13" s="25"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A14" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="J14" s="25"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1">
+      <c r="A15" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="B15" s="10">
         <v>21.1</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D15" s="10">
         <f>B15/2.20462</f>
         <v>9.5708103890919993</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F15" s="10">
         <v>156.30000000000001</v>
@@ -1769,32 +1737,32 @@
         <v>70.896571744790492</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J15" s="18">
-        <f>D15*conversion!B23/conversion!C13</f>
+        <v>80</v>
+      </c>
+      <c r="J15" s="25">
+        <f>D15/conversion!C13</f>
         <v>3.0461949575680598</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B16" s="10">
         <v>18.399999999999999</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" s="10">
         <f>B16/2.20462</f>
         <v>8.3461095336157705</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F16" s="10">
         <v>152.6</v>
@@ -1802,34 +1770,36 @@
       <c r="G16" s="10">
         <v>69.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-    </row>
-    <row r="18" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="25"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A17" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="J17" s="25"/>
+    </row>
+    <row r="18" spans="1:11" ht="22.5" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" s="10">
         <v>120.7</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="10">
         <f>B18/2.20462</f>
         <v>54.748664168881717</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F18" s="10">
         <v>120.6</v>
@@ -1838,23 +1808,24 @@
         <f>(F18/2.20462)</f>
         <v>54.703304877938152</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>46</v>
+      <c r="J18" s="25"/>
+    </row>
+    <row r="19" spans="1:11" ht="15">
+      <c r="A19" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="B19" s="10">
         <v>32.4</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D19" s="10">
         <f>B19/2.20462</f>
         <v>14.696410265714727</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F19" s="10">
         <v>225.1</v>
@@ -1864,33 +1835,33 @@
         <v>102.10376391396251</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J19" s="18">
-        <f>D19*conversion!B21/conversion!C12</f>
-        <v>4.0271495041319945</v>
-      </c>
-      <c r="K19" s="23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="J19" s="25">
+        <f>D19/conversion!C12</f>
+        <v>4.3868730981830009</v>
+      </c>
+      <c r="K19" s="21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="25">
       <c r="A20" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" s="10">
         <f>F20*5.796/42</f>
         <v>22.093800000000002</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D20" s="10">
         <f>B20/2.20462</f>
         <v>10.021591022489138</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F20" s="10">
         <v>160.1</v>
@@ -1899,35 +1870,37 @@
         <f>(F20/2.20462)</f>
         <v>72.620224800645914</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J20" s="25"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A21" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="J21" s="25"/>
+    </row>
+    <row r="22" spans="1:11" ht="15">
       <c r="A22" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B22" s="10">
         <f>F22*6.636/42</f>
         <v>26.3386</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D22" s="10">
         <f>B22/2.20462</f>
         <v>11.94700220446154</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F22" s="10">
         <v>166.7</v>
@@ -1936,24 +1909,25 @@
         <f>(F22/2.20462)</f>
         <v>75.613938002921145</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
-        <v>50</v>
+      <c r="J22" s="25"/>
+    </row>
+    <row r="23" spans="1:11" ht="15">
+      <c r="A23" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="B23" s="10">
         <f>F23*6.065/42</f>
         <v>23.624619047619049</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D23" s="10">
         <f>B23/2.20462</f>
         <v>10.715959688118158</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F23" s="10">
         <v>163.6</v>
@@ -1962,25 +1936,26 @@
         <f>(F23/2.20462)</f>
         <v>74.207799983670654</v>
       </c>
-      <c r="K23" s="23"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J23" s="25"/>
+      <c r="K23" s="21"/>
+    </row>
+    <row r="24" spans="1:11" ht="15">
       <c r="A24" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B24" s="10">
         <f>F24*6.636/42</f>
         <v>24.742799999999999</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D24" s="10">
         <f>B24/2.20462</f>
         <v>11.223158639584147</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F24" s="10">
         <v>156.6</v>
@@ -1989,24 +1964,25 @@
         <f>(F24/2.20462)</f>
         <v>71.032649617621175</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="J24" s="25"/>
+    </row>
+    <row r="25" spans="1:11" ht="15">
       <c r="A25" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" s="10">
         <f>F25*5.248/42</f>
         <v>20.054857142857145</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D25" s="10">
         <f>B25/2.20462</f>
         <v>9.0967409997446946</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F25" s="10">
         <v>160.5</v>
@@ -2015,24 +1991,25 @@
         <f>(F25/2.20462)</f>
         <v>72.801661964420177</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J25" s="25"/>
+    </row>
+    <row r="26" spans="1:11" ht="15">
       <c r="A26" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26" s="10">
         <f>F26*5.537/42</f>
         <v>21.106516666666668</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D26" s="10">
         <f>B26/2.20462</f>
         <v>9.5737663028851543</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F26" s="10">
         <v>160.1</v>
@@ -2041,34 +2018,36 @@
         <f>(F26/2.20462)</f>
         <v>72.620224800645914</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J26" s="25"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A27" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="J27" s="25"/>
+    </row>
+    <row r="28" spans="1:11" ht="15">
       <c r="A28" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28" s="10">
         <v>5685</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D28" s="10">
         <f>B28/2.20462</f>
         <v>2578.675690141612</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F28" s="10">
         <v>228.6</v>
@@ -2076,23 +2055,24 @@
       <c r="G28" s="10">
         <v>103.7</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J28" s="25"/>
+    </row>
+    <row r="29" spans="1:11" ht="15">
       <c r="A29" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="10">
         <v>4931.3</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D29" s="10">
         <f>B29/2.20462</f>
         <v>2236.8027142999704</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F29" s="10">
         <v>205.7</v>
@@ -2100,23 +2080,24 @@
       <c r="G29" s="10">
         <v>93.3</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J29" s="25"/>
+    </row>
+    <row r="30" spans="1:11" ht="15">
       <c r="A30" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B30" s="10">
         <v>3715.9</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D30" s="10">
         <f>B30/2.20462</f>
         <v>1685.5058921718937</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F30" s="10">
         <v>214.3</v>
@@ -2124,23 +2105,24 @@
       <c r="G30" s="10">
         <v>97.2</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J30" s="25"/>
+    </row>
+    <row r="31" spans="1:11" ht="15">
       <c r="A31" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B31" s="10">
         <v>2791.6</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D31" s="10">
         <f>B31/2.20462</f>
         <v>1266.2499659805319</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F31" s="10">
         <v>215.4</v>
@@ -2149,24 +2131,25 @@
         <f>(F31/2.20462)</f>
         <v>97.703912692436802</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
-        <v>59</v>
+      <c r="J31" s="25"/>
+    </row>
+    <row r="32" spans="1:11" ht="15">
+      <c r="A32" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="B32" s="11">
         <f>F32*24.8</f>
         <v>6239.68</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D32" s="11">
         <f>B32/2.20462</f>
         <v>2830.2746051473728</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F32" s="11">
         <v>251.6</v>
@@ -2176,19 +2159,19 @@
         <v>114.12397601400696</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="J32" s="18">
-        <f>D32*conversion!B20/(1000*conversion!B4)</f>
-        <v>3.0636890225739433</v>
+        <v>81</v>
+      </c>
+      <c r="J32" s="25">
+        <f>D32/(1000*conversion!B4)</f>
+        <v>3.1198462551669484</v>
       </c>
       <c r="K32" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15">
       <c r="A33" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -2196,17 +2179,18 @@
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
-    </row>
-    <row r="34" spans="1:11" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="J33" s="25"/>
+    </row>
+    <row r="34" spans="1:11" ht="25">
       <c r="A34" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11">
@@ -2217,22 +2201,22 @@
         <v>7.7065435313115183</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B35" s="11">
         <v>5771</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D35" s="11">
         <f>B35/2.20462</f>
         <v>2617.6846803530771</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F35" s="11">
         <v>91.9</v>
@@ -2242,22 +2226,22 @@
         <v>41.685188377135297</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B36" s="11">
         <v>6160</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D36" s="11">
         <f>B36/2.20462</f>
         <v>2794.1323221235407</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F36" s="11">
         <v>189.54</v>
@@ -2267,23 +2251,23 @@
         <v>85.974000054431158</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="15" thickBot="1">
       <c r="A37" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B37" s="14">
         <f>F37*4.4</f>
         <v>924.00000000000011</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D37" s="11">
         <f>B37/2.20462</f>
         <v>419.11984831853118</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F37" s="15">
         <v>210</v>
@@ -2293,50 +2277,50 @@
         <v>95.254510981484344</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
+    <row r="38" spans="1:11" ht="13.5" customHeight="1">
+      <c r="A38" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+    </row>
+    <row r="39" spans="1:11" ht="11.25" customHeight="1">
+      <c r="A39" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="K39" s="21"/>
+    </row>
+    <row r="40" spans="1:11" ht="12.75" customHeight="1">
+      <c r="A40" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-    </row>
-    <row r="39" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="K39" s="23"/>
-    </row>
-    <row r="40" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-    </row>
-    <row r="41" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+    </row>
+    <row r="41" spans="1:11" ht="24" customHeight="1">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-    </row>
-    <row r="42" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+    </row>
+    <row r="42" spans="1:11" ht="12" customHeight="1">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2345,9 +2329,9 @@
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -2371,6 +2355,204 @@
     <hyperlink ref="A43" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1">
+        <v>1055870</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2">
+        <f>10^6</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3">
+        <f>10^9</f>
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4">
+        <v>0.90718399999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5">
+        <v>3.6640000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
+        <v>29307600000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7">
+        <v>3.7854099999999999E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12">
+        <f>(800+970)/2</f>
+        <v>885</v>
+      </c>
+      <c r="C12">
+        <f>B12*$B$7</f>
+        <v>3.35008785</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13">
+        <f>(800+860)/2</f>
+        <v>830</v>
+      </c>
+      <c r="C13">
+        <f>B13*$B$7</f>
+        <v>3.1418903</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14">
+        <f>(710+790)/2</f>
+        <v>750</v>
+      </c>
+      <c r="C14">
+        <f>B14*$B$7</f>
+        <v>2.8390575</v>
+      </c>
+      <c r="D14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <f>0.982</f>
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>0.98499999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <f>0.98</f>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2381,193 +2563,491 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1">
-        <v>1055870</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2">
-        <f>10^6</f>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CDIAC!F2</f>
+        <v>kt CO2/kJ</v>
+      </c>
+      <c r="E2" s="1">
+        <f>CDIAC!G2</f>
+        <v>9.2185426472586756E-11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3">
-        <f>10^9</f>
-        <v>1000000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="str">
+        <f>CDIAC!F2</f>
+        <v>kt CO2/kJ</v>
+      </c>
+      <c r="E3" s="1">
+        <f>CDIAC!G2</f>
+        <v>9.2185426472586756E-11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4">
-        <v>0.90718399999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f>CDIAC!F4</f>
+        <v>kt CO2/TJ</v>
+      </c>
+      <c r="E4">
+        <f>CDIAC!G4</f>
+        <v>5.0196800000000007E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f>CDIAC!F5</f>
+        <v>kt CO2/kt</v>
+      </c>
+      <c r="E5">
+        <f>CDIAC!G5</f>
+        <v>3.1327199999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f>CDIAC!F6</f>
+        <v>kt CO2/TJ</v>
+      </c>
+      <c r="E6">
+        <f>CDIAC!G6</f>
+        <v>4.9295456000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f>EIA!K8</f>
+        <v>kt CO2/kt</v>
+      </c>
+      <c r="E7">
+        <f>EIA!J12</f>
+        <v>3.1314691671227299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
         <v>74</v>
       </c>
-      <c r="B5">
-        <v>3.6640000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1">
-        <v>29307600000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7">
-        <v>3.7854099999999999E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f>EIA!J8</f>
+        <v>3.2338752156172763</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" t="str">
+        <f>EIA!K19</f>
+        <v>kt CO2/kt</v>
+      </c>
+      <c r="E9">
+        <f>EIA!J19</f>
+        <v>4.3868730981830009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="str">
+        <f>EIA!K32</f>
+        <v>kt CO2/kt</v>
+      </c>
+      <c r="E10">
+        <f>EIA!J32</f>
+        <v>3.1198462551669484</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="24" t="str">
+        <f>EIA!K15</f>
+        <v>kt CO2/kt</v>
+      </c>
+      <c r="E11" s="24">
+        <f>EIA!J$8</f>
+        <v>3.2338752156172763</v>
+      </c>
+      <c r="F11" s="24"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12">
-        <f>(800+970)/2</f>
-        <v>885</v>
-      </c>
-      <c r="C12">
-        <f>B12*$B$7</f>
-        <v>3.35008785</v>
-      </c>
-      <c r="D12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="24">
+        <f>EIA!J$8</f>
+        <v>3.2338752156172763</v>
+      </c>
+      <c r="F12" s="24"/>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13">
-        <f>(800+860)/2</f>
-        <v>830</v>
-      </c>
-      <c r="C13">
-        <f>B13*$B$7</f>
-        <v>3.1418903</v>
-      </c>
-      <c r="D13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="B13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="24">
+        <f>CDIAC!G5</f>
+        <v>3.1327199999999999</v>
+      </c>
+      <c r="F13" s="24"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14">
-        <f>(710+790)/2</f>
-        <v>750</v>
-      </c>
-      <c r="C14">
-        <f>B14*$B$7</f>
-        <v>2.8390575</v>
-      </c>
-      <c r="D14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20">
-        <f>0.982</f>
-        <v>0.98199999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21">
-        <f>0.918</f>
-        <v>0.91800000000000004</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22">
-        <f>0.98</f>
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="24">
+        <f>CDIAC!G5</f>
+        <v>3.1327199999999999</v>
+      </c>
+      <c r="F14" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="23">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="23">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="23">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="23">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="E5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="23">
+        <v>0.98499999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="23">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.98</v>
+      </c>
+      <c r="E8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="23">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="23">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="23">
+        <v>0.96</v>
+      </c>
+      <c r="E11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="23">
+        <v>0.96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated EF file with additional comparisons and additional EF for coal gases.
</commit_message>
<xml_diff>
--- a/input/default-emissions-data/CO2_base_EF.xlsx
+++ b/input/default-emissions-data/CO2_base_EF.xlsx
@@ -1,10 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13740" yWindow="620" windowWidth="16020" windowHeight="14180" tabRatio="881" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="23380" windowHeight="10880" tabRatio="881" activeTab="3"/>
+    <workbookView xWindow="17860" yWindow="360" windowWidth="9380" windowHeight="9920" tabRatio="500" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="11660" yWindow="2100" windowWidth="8400" windowHeight="12120" tabRatio="500" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CDIAC" sheetId="2" r:id="rId1"/>
@@ -13,6 +15,9 @@
     <sheet name="Emission_Coefficient" sheetId="6" r:id="rId4"/>
     <sheet name="Fraction_Oxidized" sheetId="7" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="CO2_to_C">conversion!$B$5</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -22,8 +27,90 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Steve Smith</author>
+  </authors>
+  <commentList>
+    <comment ref="P3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Smith:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Sub-bituminous</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Smith:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+S</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Steve Smith:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+From guideline doc, is TJ Net</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="123">
   <si>
     <t>cdiac_fuel</t>
   </si>
@@ -356,16 +443,53 @@
   </si>
   <si>
     <t>discussed in data and assumptions supplement</t>
+  </si>
+  <si>
+    <t>EC (kg/GJ)</t>
+  </si>
+  <si>
+    <t>IPCC_2008</t>
+  </si>
+  <si>
+    <t>IPCC_1996</t>
+  </si>
+  <si>
+    <t>IPCC_1996 (kgC/GJ)</t>
+  </si>
+  <si>
+    <t>gas_works_gas</t>
+  </si>
+  <si>
+    <t>coke_oven_gas</t>
+  </si>
+  <si>
+    <t>blast_furnace_gas</t>
+  </si>
+  <si>
+    <t>oxygen_steel_furnace_gas</t>
+  </si>
+  <si>
+    <t>IPCC_96_diff</t>
+  </si>
+  <si>
+    <t>IPCC_08_diff</t>
+  </si>
+  <si>
+    <t>1A1b_Mass_Balance_Adjust</t>
+  </si>
+  <si>
+    <t>kgCO2/GJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -469,6 +593,32 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -592,7 +742,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="82">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -696,8 +846,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -754,6 +951,16 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="24" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="54"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="82" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="28" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -776,7 +983,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="82">
+  <cellStyles count="129">
     <cellStyle name="Body: normal cell" xfId="25"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -835,6 +1042,52 @@
     <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Font: Calibri, 9pt regular" xfId="30"/>
     <cellStyle name="Footnotes: all except top row" xfId="31"/>
     <cellStyle name="Footnotes: top row" xfId="28"/>
@@ -856,6 +1109,7 @@
     <cellStyle name="Normal 2" xfId="24"/>
     <cellStyle name="Output" xfId="54" builtinId="21"/>
     <cellStyle name="Parent row" xfId="26"/>
+    <cellStyle name="Percent" xfId="82" builtinId="5"/>
     <cellStyle name="Section Break" xfId="33"/>
     <cellStyle name="Section Break: parent row" xfId="34"/>
     <cellStyle name="Table title" xfId="23"/>
@@ -1195,10 +1449,15 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="7" max="7" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
@@ -1359,6 +1618,8 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -1369,34 +1630,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+    <sheetView workbookViewId="2">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19" style="3" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.375" style="3" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="17" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="17" customWidth="1"/>
-    <col min="8" max="9" width="8.83203125" style="3"/>
-    <col min="10" max="11" width="8.83203125" style="18"/>
-    <col min="12" max="16384" width="8.83203125" style="3"/>
+    <col min="7" max="7" width="11.625" style="17" customWidth="1"/>
+    <col min="8" max="9" width="8.875" style="3"/>
+    <col min="10" max="11" width="8.875" style="18"/>
+    <col min="12" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1">
       <c r="A2" s="4"/>
@@ -1438,18 +1705,18 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="J4" s="25"/>
     </row>
-    <row r="5" spans="1:11" ht="15">
+    <row r="5" spans="1:11" ht="16">
       <c r="A5" s="10" t="s">
         <v>27</v>
       </c>
@@ -1475,7 +1742,7 @@
       </c>
       <c r="J5" s="25"/>
     </row>
-    <row r="6" spans="1:11" ht="15">
+    <row r="6" spans="1:11" ht="16">
       <c r="A6" s="10" t="s">
         <v>29</v>
       </c>
@@ -1562,7 +1829,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15">
+    <row r="9" spans="1:11" ht="16">
       <c r="A9" s="10" t="s">
         <v>32</v>
       </c>
@@ -1588,7 +1855,7 @@
       </c>
       <c r="J9" s="25"/>
     </row>
-    <row r="10" spans="1:11" ht="15">
+    <row r="10" spans="1:11" ht="16">
       <c r="A10" s="10" t="s">
         <v>33</v>
       </c>
@@ -1614,7 +1881,7 @@
       </c>
       <c r="J10" s="25"/>
     </row>
-    <row r="11" spans="1:11" ht="25">
+    <row r="11" spans="1:11" ht="27">
       <c r="A11" s="10" t="s">
         <v>35</v>
       </c>
@@ -1674,7 +1941,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="25">
+    <row r="13" spans="1:11" ht="27">
       <c r="A13" s="10" t="s">
         <v>38</v>
       </c>
@@ -1701,15 +1968,15 @@
       <c r="J13" s="25"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
       <c r="J14" s="25"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
@@ -1747,7 +2014,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15">
+    <row r="16" spans="1:11" ht="16">
       <c r="A16" s="10" t="s">
         <v>41</v>
       </c>
@@ -1773,15 +2040,15 @@
       <c r="J16" s="25"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
       <c r="J17" s="25"/>
     </row>
     <row r="18" spans="1:11" ht="22.5" customHeight="1">
@@ -1810,7 +2077,7 @@
       </c>
       <c r="J18" s="25"/>
     </row>
-    <row r="19" spans="1:11" ht="15">
+    <row r="19" spans="1:11" ht="16">
       <c r="A19" s="19" t="s">
         <v>44</v>
       </c>
@@ -1845,7 +2112,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="25">
+    <row r="20" spans="1:11" ht="27">
       <c r="A20" s="10" t="s">
         <v>45</v>
       </c>
@@ -1873,18 +2140,18 @@
       <c r="J20" s="25"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
       <c r="J21" s="25"/>
     </row>
-    <row r="22" spans="1:11" ht="15">
+    <row r="22" spans="1:11" ht="16">
       <c r="A22" s="10" t="s">
         <v>47</v>
       </c>
@@ -1911,7 +2178,7 @@
       </c>
       <c r="J22" s="25"/>
     </row>
-    <row r="23" spans="1:11" ht="15">
+    <row r="23" spans="1:11" ht="16">
       <c r="A23" s="22" t="s">
         <v>48</v>
       </c>
@@ -1939,7 +2206,7 @@
       <c r="J23" s="25"/>
       <c r="K23" s="21"/>
     </row>
-    <row r="24" spans="1:11" ht="15">
+    <row r="24" spans="1:11" ht="16">
       <c r="A24" s="10" t="s">
         <v>49</v>
       </c>
@@ -1966,7 +2233,7 @@
       </c>
       <c r="J24" s="25"/>
     </row>
-    <row r="25" spans="1:11" ht="15">
+    <row r="25" spans="1:11" ht="16">
       <c r="A25" s="10" t="s">
         <v>50</v>
       </c>
@@ -1993,7 +2260,7 @@
       </c>
       <c r="J25" s="25"/>
     </row>
-    <row r="26" spans="1:11" ht="15">
+    <row r="26" spans="1:11" ht="16">
       <c r="A26" s="10" t="s">
         <v>51</v>
       </c>
@@ -2021,18 +2288,18 @@
       <c r="J26" s="25"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
       <c r="J27" s="25"/>
     </row>
-    <row r="28" spans="1:11" ht="15">
+    <row r="28" spans="1:11" ht="16">
       <c r="A28" s="10" t="s">
         <v>53</v>
       </c>
@@ -2057,7 +2324,7 @@
       </c>
       <c r="J28" s="25"/>
     </row>
-    <row r="29" spans="1:11" ht="15">
+    <row r="29" spans="1:11" ht="16">
       <c r="A29" s="10" t="s">
         <v>54</v>
       </c>
@@ -2082,7 +2349,7 @@
       </c>
       <c r="J29" s="25"/>
     </row>
-    <row r="30" spans="1:11" ht="15">
+    <row r="30" spans="1:11" ht="16">
       <c r="A30" s="10" t="s">
         <v>55</v>
       </c>
@@ -2107,7 +2374,7 @@
       </c>
       <c r="J30" s="25"/>
     </row>
-    <row r="31" spans="1:11" ht="15">
+    <row r="31" spans="1:11" ht="16">
       <c r="A31" s="10" t="s">
         <v>56</v>
       </c>
@@ -2133,7 +2400,7 @@
       </c>
       <c r="J31" s="25"/>
     </row>
-    <row r="32" spans="1:11" ht="15">
+    <row r="32" spans="1:11" ht="16">
       <c r="A32" s="20" t="s">
         <v>57</v>
       </c>
@@ -2169,7 +2436,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15">
+    <row r="33" spans="1:11" ht="16">
       <c r="A33" s="12" t="s">
         <v>58</v>
       </c>
@@ -2181,7 +2448,7 @@
       <c r="G33" s="11"/>
       <c r="J33" s="25"/>
     </row>
-    <row r="34" spans="1:11" ht="25">
+    <row r="34" spans="1:11" ht="27">
       <c r="A34" s="11" t="s">
         <v>59</v>
       </c>
@@ -2251,7 +2518,7 @@
         <v>85.974000054431158</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15" thickBot="1">
+    <row r="37" spans="1:11" ht="16" thickBot="1">
       <c r="A37" s="4" t="s">
         <v>63</v>
       </c>
@@ -2278,47 +2545,47 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
     </row>
     <row r="39" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
       <c r="K39" s="21"/>
     </row>
     <row r="40" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
     </row>
     <row r="41" spans="1:11" ht="24" customHeight="1">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
     </row>
     <row r="42" spans="1:11" ht="12" customHeight="1">
       <c r="A42" s="4"/>
@@ -2359,6 +2626,8 @@
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
@@ -2369,10 +2638,14 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="2">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -2555,6 +2828,8 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -2562,19 +2837,31 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="8.875" customWidth="1"/>
+    <col min="11" max="11" width="7.625" customWidth="1"/>
+    <col min="12" max="12" width="3.125" customWidth="1"/>
+    <col min="15" max="15" width="3.125" customWidth="1"/>
+    <col min="16" max="16" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -2590,8 +2877,32 @@
       <c r="E1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="P1" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>112</v>
+      </c>
+      <c r="R1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -2609,8 +2920,25 @@
         <f>CDIAC!G2</f>
         <v>9.2185426472586756E-11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2" s="26">
+        <f>IF(D2="kt CO2/kJ",E2*1000000*1000000,"")</f>
+        <v>92.185426472586755</v>
+      </c>
+      <c r="I2" s="26">
+        <f>P2*CO2_to_C</f>
+        <v>94.531200000000013</v>
+      </c>
+      <c r="M2" s="28">
+        <f>(H2-I2)/I2</f>
+        <v>-2.4814807464765675E-2</v>
+      </c>
+      <c r="P2" s="27">
+        <v>25.8</v>
+      </c>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -2628,8 +2956,35 @@
         <f>CDIAC!G2</f>
         <v>9.2185426472586756E-11</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3" s="26">
+        <f t="shared" ref="H3:H14" si="0">IF(D3="kt CO2/kJ",E3*1000000*1000000,"")</f>
+        <v>92.185426472586755</v>
+      </c>
+      <c r="I3" s="26">
+        <f>P3*CO2_to_C</f>
+        <v>95.996800000000007</v>
+      </c>
+      <c r="K3" s="26">
+        <f>S3*CO2_to_C</f>
+        <v>101.1264</v>
+      </c>
+      <c r="L3" s="26"/>
+      <c r="M3" s="28">
+        <f>(H3-I3)/I3</f>
+        <v>-3.9703131014921872E-2</v>
+      </c>
+      <c r="N3" s="28"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26">
+        <f>26.2</f>
+        <v>26.2</v>
+      </c>
+      <c r="Q3" s="27"/>
+      <c r="S3" s="26">
+        <v>27.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -2647,8 +3002,31 @@
         <f>CDIAC!G4</f>
         <v>5.0196800000000007E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4" s="26">
+        <f>IF(D4="kt CO2/TJ",E4/1000*1000000,"")</f>
+        <v>50.19680000000001</v>
+      </c>
+      <c r="I4" s="26">
+        <f>P4*CO2_to_C</f>
+        <v>56.1</v>
+      </c>
+      <c r="M4" s="28">
+        <f>(H4-I4)/I4</f>
+        <v>-0.10522638146167541</v>
+      </c>
+      <c r="P4" s="26">
+        <f>Q4</f>
+        <v>15.31113537117904</v>
+      </c>
+      <c r="Q4" s="26">
+        <f>R4/CO2_to_C</f>
+        <v>15.31113537117904</v>
+      </c>
+      <c r="R4" s="27">
+        <v>56.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>98</v>
       </c>
@@ -2666,8 +3044,12 @@
         <f>CDIAC!G5</f>
         <v>3.1327199999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="H5" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -2685,8 +3067,12 @@
         <f>CDIAC!G6</f>
         <v>4.9295456000000001E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6" s="26">
+        <f>IF(D6="kt CO2/TJ",E6/1000*1000000,"")</f>
+        <v>49.295456000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -2704,8 +3090,12 @@
         <f>EIA!J12</f>
         <v>3.1314691671227299</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="H7" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -2722,8 +3112,12 @@
         <f>EIA!J8</f>
         <v>3.2338752156172763</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="H8" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -2741,8 +3135,12 @@
         <f>EIA!J19</f>
         <v>4.3868730981830009</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="H9" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -2760,8 +3158,12 @@
         <f>EIA!J32</f>
         <v>3.1198462551669484</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="H10" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>98</v>
       </c>
@@ -2780,8 +3182,12 @@
         <v>3.2338752156172763</v>
       </c>
       <c r="F11" s="24"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="H11" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -2799,8 +3205,12 @@
         <v>3.2338752156172763</v>
       </c>
       <c r="F12" s="24"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="H12" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -2818,8 +3228,12 @@
         <v>3.1327199999999999</v>
       </c>
       <c r="F13" s="24"/>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="H13" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>98</v>
       </c>
@@ -2837,12 +3251,119 @@
         <v>3.1327199999999999</v>
       </c>
       <c r="F14" s="24"/>
+      <c r="H14" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15">
+        <f>Q15*CO2_to_C/1000</f>
+        <v>4.4400000000000002E-2</v>
+      </c>
+      <c r="Q15" s="26">
+        <f>R15/CO2_to_C</f>
+        <v>12.117903930131003</v>
+      </c>
+      <c r="R15" s="27">
+        <v>44.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16">
+        <f>Q16*CO2_to_C/1000</f>
+        <v>4.4400000000000002E-2</v>
+      </c>
+      <c r="Q16" s="26">
+        <f>R16/CO2_to_C</f>
+        <v>12.117903930131003</v>
+      </c>
+      <c r="R16" s="27">
+        <v>44.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17">
+        <f>Q17*CO2_to_C/1000</f>
+        <v>0.26</v>
+      </c>
+      <c r="Q17" s="26">
+        <f>R17/CO2_to_C</f>
+        <v>70.960698689956331</v>
+      </c>
+      <c r="R17" s="27">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18">
+        <f>Q18*CO2_to_C/1000</f>
+        <v>0.182</v>
+      </c>
+      <c r="Q18" s="26">
+        <f>R18/CO2_to_C</f>
+        <v>49.672489082969427</v>
+      </c>
+      <c r="R18" s="27">
+        <v>182</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -2853,11 +3374,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -3051,6 +3574,8 @@
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
Update CO2 Emissions assumptions and data (#236)
* Update USGS cement data (although future revisions may use use Andrews data instead)
* Update default CO2 heavy oil combustion EFs
* Replace default CO2 combustion EFs with maximum possible values (by CEDS_fuel)
* Remove UNFCCC CO2 scaling & add UNFCCC flaring CO2 emissions into default data instead
</commit_message>
<xml_diff>
--- a/input/default-emissions-data/CO2_base_EF.xlsx
+++ b/input/default-emissions-data/CO2_base_EF.xlsx
@@ -1,12 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Documents/Information &amp; Documents/CEDS_Project/CEDS/input/default-emissions-data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6F7AB3-2DC4-7D4F-B18F-6DED73BF7E5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="23380" windowHeight="10880" tabRatio="881" activeTab="3"/>
-    <workbookView xWindow="17860" yWindow="360" windowWidth="9380" windowHeight="9920" tabRatio="500" firstSheet="3" activeTab="3"/>
-    <workbookView xWindow="11660" yWindow="2100" windowWidth="8400" windowHeight="12120" tabRatio="500" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="23380" windowHeight="10880" tabRatio="881" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6600" yWindow="4620" windowWidth="20160" windowHeight="12700" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
+    <workbookView xWindow="1580" yWindow="460" windowWidth="20020" windowHeight="13260" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF02000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CDIAC" sheetId="2" r:id="rId1"/>
@@ -18,8 +24,16 @@
   <definedNames>
     <definedName name="CO2_to_C">conversion!$B$5</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,12 +42,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Steve Smith</author>
   </authors>
   <commentList>
-    <comment ref="P3" authorId="0">
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="0">
+    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -81,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R4" authorId="0">
+    <comment ref="R4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -110,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="125">
   <si>
     <t>cdiac_fuel</t>
   </si>
@@ -479,17 +493,23 @@
   </si>
   <si>
     <t>kgCO2/GJ</t>
+  </si>
+  <si>
+    <t>From: US GHG inventory 2019, Table A-23, 85.68% carbon content of residual oil</t>
+  </si>
+  <si>
+    <t>Carbon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -563,17 +583,20 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -594,6 +617,7 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -620,10 +644,18 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -633,6 +665,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -894,7 +932,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -961,6 +999,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="28" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -982,9 +1021,10 @@
     <xf numFmtId="4" fontId="7" fillId="0" borderId="4" xfId="26" applyNumberFormat="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="82" applyFont="1"/>
   </cellXfs>
   <cellStyles count="129">
-    <cellStyle name="Body: normal cell" xfId="25"/>
+    <cellStyle name="Body: normal cell" xfId="25" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1088,11 +1128,11 @@
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="30"/>
-    <cellStyle name="Footnotes: all except top row" xfId="31"/>
-    <cellStyle name="Footnotes: top row" xfId="28"/>
-    <cellStyle name="Header: bottom row" xfId="27"/>
-    <cellStyle name="Header: top rows" xfId="32"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="30" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Footnotes: all except top row" xfId="31" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="28" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Header: bottom row" xfId="27" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Header: top rows" xfId="32" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1106,19 +1146,22 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="24"/>
+    <cellStyle name="Normal 2" xfId="24" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
     <cellStyle name="Output" xfId="54" builtinId="21"/>
-    <cellStyle name="Parent row" xfId="26"/>
+    <cellStyle name="Parent row" xfId="26" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
     <cellStyle name="Percent" xfId="82" builtinId="5"/>
-    <cellStyle name="Section Break" xfId="33"/>
-    <cellStyle name="Section Break: parent row" xfId="34"/>
-    <cellStyle name="Table title" xfId="23"/>
+    <cellStyle name="Section Break" xfId="33" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Section Break: parent row" xfId="34" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Table title" xfId="23" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1445,21 +1488,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="2">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1482,7 +1527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1507,7 +1552,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1533,7 +1578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1559,7 +1604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1585,7 +1630,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1611,7 +1656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D9" s="1"/>
     </row>
   </sheetData>
@@ -1627,45 +1672,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="1">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
     <sheetView workbookViewId="2">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" style="3" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="17" customWidth="1"/>
-    <col min="7" max="7" width="11.625" style="17" customWidth="1"/>
-    <col min="8" max="9" width="8.875" style="3"/>
-    <col min="10" max="11" width="8.875" style="18"/>
-    <col min="12" max="16384" width="8.875" style="3"/>
+    <col min="7" max="7" width="11.6640625" style="17" customWidth="1"/>
+    <col min="8" max="9" width="8.83203125" style="3"/>
+    <col min="10" max="11" width="8.83203125" style="18"/>
+    <col min="12" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" customHeight="1">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-    </row>
-    <row r="2" spans="1:11" ht="30" customHeight="1">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>20</v>
@@ -1682,7 +1727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="27.75" customHeight="1" thickBot="1">
+    <row r="3" spans="1:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
@@ -1704,19 +1749,19 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A4" s="34" t="s">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
       <c r="J4" s="25"/>
     </row>
-    <row r="5" spans="1:11" ht="16">
+    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>27</v>
       </c>
@@ -1742,7 +1787,7 @@
       </c>
       <c r="J5" s="25"/>
     </row>
-    <row r="6" spans="1:11" ht="16">
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>29</v>
       </c>
@@ -1768,7 +1813,7 @@
       </c>
       <c r="J6" s="25"/>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1">
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>30</v>
       </c>
@@ -1794,7 +1839,7 @@
       </c>
       <c r="J7" s="25"/>
     </row>
-    <row r="8" spans="1:11" ht="26.25" customHeight="1">
+    <row r="8" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>31</v>
       </c>
@@ -1829,7 +1874,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16">
+    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>32</v>
       </c>
@@ -1855,7 +1900,7 @@
       </c>
       <c r="J9" s="25"/>
     </row>
-    <row r="10" spans="1:11" ht="16">
+    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>33</v>
       </c>
@@ -1879,9 +1924,22 @@
         <f t="shared" si="1"/>
         <v>95.345229563371475</v>
       </c>
-      <c r="J10" s="25"/>
-    </row>
-    <row r="11" spans="1:11" ht="27">
+      <c r="J10" s="25">
+        <f>B10/2000</f>
+        <v>2.31575</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="L10" s="38">
+        <f>EIA!B10/2000/((15.9994*2+12.011)/12.011)</f>
+        <v>0.63200635426654972</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="27" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>35</v>
       </c>
@@ -1907,7 +1965,7 @@
       </c>
       <c r="J11" s="25"/>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1">
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>37</v>
       </c>
@@ -1941,7 +1999,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="27">
+    <row r="13" spans="1:13" ht="27" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>38</v>
       </c>
@@ -1967,19 +2025,19 @@
       </c>
       <c r="J13" s="25"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A14" s="35" t="s">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
       <c r="J14" s="25"/>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1">
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>40</v>
       </c>
@@ -2014,7 +2072,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="16">
+    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>41</v>
       </c>
@@ -2039,19 +2097,19 @@
       </c>
       <c r="J16" s="25"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A17" s="35" t="s">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
       <c r="J17" s="25"/>
     </row>
-    <row r="18" spans="1:11" ht="22.5" customHeight="1">
+    <row r="18" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>43</v>
       </c>
@@ -2077,7 +2135,7 @@
       </c>
       <c r="J18" s="25"/>
     </row>
-    <row r="19" spans="1:11" ht="16">
+    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>44</v>
       </c>
@@ -2104,15 +2162,10 @@
       <c r="H19" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="J19" s="25">
-        <f>D19/conversion!C12</f>
-        <v>4.3868730981830009</v>
-      </c>
-      <c r="K19" s="21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="27">
+      <c r="J19" s="25"/>
+      <c r="K19" s="21"/>
+    </row>
+    <row r="20" spans="1:11" ht="27" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>45</v>
       </c>
@@ -2139,19 +2192,19 @@
       </c>
       <c r="J20" s="25"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="35" t="s">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
       <c r="J21" s="25"/>
     </row>
-    <row r="22" spans="1:11" ht="16">
+    <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>47</v>
       </c>
@@ -2178,7 +2231,7 @@
       </c>
       <c r="J22" s="25"/>
     </row>
-    <row r="23" spans="1:11" ht="16">
+    <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
         <v>48</v>
       </c>
@@ -2206,7 +2259,7 @@
       <c r="J23" s="25"/>
       <c r="K23" s="21"/>
     </row>
-    <row r="24" spans="1:11" ht="16">
+    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>49</v>
       </c>
@@ -2233,7 +2286,7 @@
       </c>
       <c r="J24" s="25"/>
     </row>
-    <row r="25" spans="1:11" ht="16">
+    <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>50</v>
       </c>
@@ -2260,7 +2313,7 @@
       </c>
       <c r="J25" s="25"/>
     </row>
-    <row r="26" spans="1:11" ht="16">
+    <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>51</v>
       </c>
@@ -2287,19 +2340,19 @@
       </c>
       <c r="J26" s="25"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="36" t="s">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
       <c r="J27" s="25"/>
     </row>
-    <row r="28" spans="1:11" ht="16">
+    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>53</v>
       </c>
@@ -2324,7 +2377,7 @@
       </c>
       <c r="J28" s="25"/>
     </row>
-    <row r="29" spans="1:11" ht="16">
+    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>54</v>
       </c>
@@ -2349,7 +2402,7 @@
       </c>
       <c r="J29" s="25"/>
     </row>
-    <row r="30" spans="1:11" ht="16">
+    <row r="30" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>55</v>
       </c>
@@ -2374,7 +2427,7 @@
       </c>
       <c r="J30" s="25"/>
     </row>
-    <row r="31" spans="1:11" ht="16">
+    <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>56</v>
       </c>
@@ -2400,7 +2453,7 @@
       </c>
       <c r="J31" s="25"/>
     </row>
-    <row r="32" spans="1:11" ht="16">
+    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
         <v>57</v>
       </c>
@@ -2436,7 +2489,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="16">
+    <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>58</v>
       </c>
@@ -2448,7 +2501,7 @@
       <c r="G33" s="11"/>
       <c r="J33" s="25"/>
     </row>
-    <row r="34" spans="1:11" ht="27">
+    <row r="34" spans="1:11" ht="27" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>59</v>
       </c>
@@ -2468,7 +2521,7 @@
         <v>7.7065435313115183</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>61</v>
       </c>
@@ -2493,7 +2546,7 @@
         <v>41.685188377135297</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>62</v>
       </c>
@@ -2518,7 +2571,7 @@
         <v>85.974000054431158</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="16" thickBot="1">
+    <row r="37" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>63</v>
       </c>
@@ -2544,50 +2597,50 @@
         <v>95.254510981484344</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A38" s="30" t="s">
+    <row r="38" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-    </row>
-    <row r="39" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A39" s="31" t="s">
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+    </row>
+    <row r="39" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
       <c r="K39" s="21"/>
     </row>
-    <row r="40" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A40" s="31" t="s">
+    <row r="40" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-    </row>
-    <row r="41" spans="1:11" ht="24" customHeight="1">
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+    </row>
+    <row r="41" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-    </row>
-    <row r="42" spans="1:11" ht="12" customHeight="1">
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+    </row>
+    <row r="42" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2596,7 +2649,7 @@
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
         <v>11</v>
       </c>
@@ -2619,7 +2672,7 @@
     <mergeCell ref="A27:G27"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A43" r:id="rId1"/>
+    <hyperlink ref="A43" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2634,20 +2687,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView tabSelected="1" workbookViewId="2">
+    <sheetView topLeftCell="A5" workbookViewId="2">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -2655,7 +2708,7 @@
         <v>1055870</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -2664,7 +2717,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -2673,7 +2726,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -2681,7 +2734,7 @@
         <v>0.90718399999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -2689,7 +2742,7 @@
         <v>3.6640000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2697,7 +2750,7 @@
         <v>29307600000</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -2705,17 +2758,17 @@
         <v>3.7854099999999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -2731,7 +2784,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -2747,7 +2800,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>89</v>
       </c>
@@ -2763,7 +2816,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>85</v>
       </c>
@@ -2771,17 +2824,17 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2790,7 +2843,7 @@
         <v>0.98199999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -2798,7 +2851,7 @@
         <v>0.98499999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -2807,7 +2860,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -2815,7 +2868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -2837,7 +2890,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2846,22 +2899,24 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
-    <sheetView workbookViewId="2"/>
+    <sheetView tabSelected="1" workbookViewId="2">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="10" max="10" width="8.875" customWidth="1"/>
-    <col min="11" max="11" width="7.625" customWidth="1"/>
-    <col min="12" max="12" width="3.125" customWidth="1"/>
-    <col min="15" max="15" width="3.125" customWidth="1"/>
-    <col min="16" max="16" width="15.875" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" customWidth="1"/>
+    <col min="12" max="12" width="3.1640625" customWidth="1"/>
+    <col min="15" max="15" width="3.1640625" customWidth="1"/>
+    <col min="16" max="16" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -2902,7 +2957,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -2920,6 +2975,9 @@
         <f>CDIAC!G2</f>
         <v>9.2185426472586756E-11</v>
       </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
       <c r="H2" s="26">
         <f>IF(D2="kt CO2/kJ",E2*1000000*1000000,"")</f>
         <v>92.185426472586755</v>
@@ -2938,7 +2996,7 @@
       <c r="Q2" s="27"/>
       <c r="R2" s="27"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -2955,6 +3013,9 @@
       <c r="E3" s="1">
         <f>CDIAC!G2</f>
         <v>9.2185426472586756E-11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
       </c>
       <c r="H3" s="26">
         <f t="shared" ref="H3:H14" si="0">IF(D3="kt CO2/kJ",E3*1000000*1000000,"")</f>
@@ -2984,7 +3045,7 @@
         <v>27.6</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -3002,6 +3063,9 @@
         <f>CDIAC!G4</f>
         <v>5.0196800000000007E-2</v>
       </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
       <c r="H4" s="26">
         <f>IF(D4="kt CO2/TJ",E4/1000*1000000,"")</f>
         <v>50.19680000000001</v>
@@ -3026,7 +3090,7 @@
         <v>56.1</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>98</v>
       </c>
@@ -3044,12 +3108,15 @@
         <f>CDIAC!G5</f>
         <v>3.1327199999999999</v>
       </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
       <c r="H5" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -3067,12 +3134,15 @@
         <f>CDIAC!G6</f>
         <v>4.9295456000000001E-2</v>
       </c>
+      <c r="F6" t="s">
+        <v>75</v>
+      </c>
       <c r="H6" s="26">
         <f>IF(D6="kt CO2/TJ",E6/1000*1000000,"")</f>
         <v>49.295456000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -3090,12 +3160,15 @@
         <f>EIA!J12</f>
         <v>3.1314691671227299</v>
       </c>
+      <c r="F7" t="s">
+        <v>74</v>
+      </c>
       <c r="H7" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -3112,12 +3185,15 @@
         <f>EIA!J8</f>
         <v>3.2338752156172763</v>
       </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
       <c r="H8" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -3127,20 +3203,23 @@
       <c r="C9" t="s">
         <v>76</v>
       </c>
-      <c r="D9" t="str">
+      <c r="D9">
         <f>EIA!K19</f>
-        <v>kt CO2/kt</v>
-      </c>
-      <c r="E9">
-        <f>EIA!J19</f>
-        <v>4.3868730981830009</v>
-      </c>
-      <c r="H9" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:19">
+        <v>0</v>
+      </c>
+      <c r="E9" s="30">
+        <f>85.68%*(15.9994*2+12.011)/12.011</f>
+        <v>3.1394219165764721</v>
+      </c>
+      <c r="F9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -3158,12 +3237,15 @@
         <f>EIA!J32</f>
         <v>3.1198462551669484</v>
       </c>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
       <c r="H10" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>98</v>
       </c>
@@ -3181,13 +3263,15 @@
         <f>EIA!J$8</f>
         <v>3.2338752156172763</v>
       </c>
-      <c r="F11" s="24"/>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
       <c r="H11" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -3204,13 +3288,15 @@
         <f>EIA!J$8</f>
         <v>3.2338752156172763</v>
       </c>
-      <c r="F12" s="24"/>
+      <c r="F12" t="s">
+        <v>74</v>
+      </c>
       <c r="H12" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -3227,13 +3313,15 @@
         <f>CDIAC!G5</f>
         <v>3.1327199999999999</v>
       </c>
-      <c r="F13" s="24"/>
+      <c r="F13" t="s">
+        <v>74</v>
+      </c>
       <c r="H13" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>98</v>
       </c>
@@ -3250,13 +3338,15 @@
         <f>CDIAC!G5</f>
         <v>3.1327199999999999</v>
       </c>
-      <c r="F14" s="24"/>
+      <c r="F14" t="s">
+        <v>74</v>
+      </c>
       <c r="H14" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -3273,6 +3363,9 @@
         <f>Q15*CO2_to_C/1000</f>
         <v>4.4400000000000002E-2</v>
       </c>
+      <c r="F15" t="s">
+        <v>75</v>
+      </c>
       <c r="Q15" s="26">
         <f>R15/CO2_to_C</f>
         <v>12.117903930131003</v>
@@ -3281,7 +3374,7 @@
         <v>44.4</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>98</v>
       </c>
@@ -3298,6 +3391,9 @@
         <f>Q16*CO2_to_C/1000</f>
         <v>4.4400000000000002E-2</v>
       </c>
+      <c r="F16" t="s">
+        <v>75</v>
+      </c>
       <c r="Q16" s="26">
         <f>R16/CO2_to_C</f>
         <v>12.117903930131003</v>
@@ -3306,7 +3402,7 @@
         <v>44.4</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>98</v>
       </c>
@@ -3323,6 +3419,9 @@
         <f>Q17*CO2_to_C/1000</f>
         <v>0.26</v>
       </c>
+      <c r="F17" t="s">
+        <v>75</v>
+      </c>
       <c r="Q17" s="26">
         <f>R17/CO2_to_C</f>
         <v>70.960698689956331</v>
@@ -3331,7 +3430,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -3347,6 +3446,9 @@
       <c r="E18">
         <f>Q18*CO2_to_C/1000</f>
         <v>0.182</v>
+      </c>
+      <c r="F18" t="s">
+        <v>75</v>
       </c>
       <c r="Q18" s="26">
         <f>R18/CO2_to_C</f>
@@ -3371,18 +3473,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
+    <sheetView workbookViewId="2">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>95</v>
       </c>
@@ -3396,7 +3500,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -3413,7 +3517,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -3427,7 +3531,7 @@
         <v>0.98199999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -3441,7 +3545,7 @@
         <v>0.98199999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>98</v>
       </c>
@@ -3458,7 +3562,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -3472,7 +3576,7 @@
         <v>0.98499999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -3486,7 +3590,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -3503,7 +3607,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -3520,7 +3624,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -3537,7 +3641,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>109</v>
       </c>
@@ -3554,7 +3658,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>109</v>
       </c>

</xml_diff>